<commit_message>
Dynamic message timers and list lengths #15 Filtersize now dynamically set by TI code #16
</commit_message>
<xml_diff>
--- a/Documents/Results/Side-by-side_33IDs.xlsx
+++ b/Documents/Results/Side-by-side_33IDs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="56">
   <si>
     <t>CAN ID</t>
   </si>
@@ -179,11 +179,20 @@
   <si>
     <t>These ones were tested at the same time as their corresponding RD test</t>
   </si>
+  <si>
+    <t>No duplicates</t>
+  </si>
+  <si>
+    <t>1 duplicate</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000%"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -200,7 +209,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -210,6 +219,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -307,7 +322,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -334,6 +349,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -574,7 +592,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$AJ$4</c:f>
+              <c:f>Sheet1!$AN$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -597,7 +615,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$AJ$39</c:f>
+              <c:f>Sheet1!$AN$39</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -613,7 +631,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$AL$4</c:f>
+              <c:f>Sheet1!$AP$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -636,7 +654,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$AL$39</c:f>
+              <c:f>Sheet1!$AP$39</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -652,7 +670,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$AN$4</c:f>
+              <c:f>Sheet1!$AR$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -675,7 +693,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$AN$39</c:f>
+              <c:f>Sheet1!$AR$39</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -691,7 +709,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$AP$4</c:f>
+              <c:f>Sheet1!$AT$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -714,7 +732,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$AP$39</c:f>
+              <c:f>Sheet1!$AT$39</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -734,11 +752,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="68536960"/>
-        <c:axId val="68543232"/>
+        <c:axId val="46029440"/>
+        <c:axId val="46039808"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="68536960"/>
+        <c:axId val="46029440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -751,7 +769,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68543232"/>
+        <c:crossAx val="46039808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -759,7 +777,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68543232"/>
+        <c:axId val="46039808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -775,7 +793,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68536960"/>
+        <c:crossAx val="46029440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2006,7 +2024,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$AJ$4</c:f>
+              <c:f>Sheet1!$AN$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2125,7 +2143,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$AJ$6:$AJ$38</c:f>
+              <c:f>Sheet1!$AN$6:$AN$38</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="33"/>
@@ -2237,7 +2255,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$AL$4</c:f>
+              <c:f>Sheet1!$AP$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2356,7 +2374,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$AL$6:$AL$38</c:f>
+              <c:f>Sheet1!$AP$6:$AP$38</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="33"/>
@@ -2468,7 +2486,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$AN$4</c:f>
+              <c:f>Sheet1!$AR$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2587,7 +2605,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$AN$6:$AN$38</c:f>
+              <c:f>Sheet1!$AR$6:$AR$38</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="33"/>
@@ -2699,7 +2717,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$AP$4</c:f>
+              <c:f>Sheet1!$AT$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2818,7 +2836,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$AP$6:$AP$38</c:f>
+              <c:f>Sheet1!$AT$6:$AT$38</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="33"/>
@@ -2920,6 +2938,246 @@
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>0.73076070082058109</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:v>Remote</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Y$6:$Y$38</c:f>
+              <c:numCache>
+                <c:formatCode>0.000%</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>0.99855898197618997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.96468710514065303</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.99898027045001103</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.96404424641440001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.99909113076633194</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.96402207887211544</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99935711277128736</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.96388907361840792</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99911321967765532</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9994236311239193</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.99935714127374697</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.99953446097231147</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.9992462367260071</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.9996674794945688</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.99973398949258496</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.99829302356514216</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.99966745737912077</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.99984482376413208</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.99971182195030039</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.99960096654769559</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.9635343929418545</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.99995566098388278</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.99982265573043672</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.99995566491543086</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.99997783147487196</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.99986698295164833</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.99980048769674135</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.99995566491543086</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.99995566294974392</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.9925704147261033</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.99345752938567311</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.99478820137502777</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.99500998003992014</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AA$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1 duplicate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AA$6:$AA$38</c:f>
+              <c:numCache>
+                <c:formatCode>0.000%</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>0.99549958986410092</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99541131874709055</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.99543338505874523</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99541131874709055</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.99541131874709055</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.99541131874709055</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99545545234875521</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.99541131874709055</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99549958986410092</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.99543338505874523</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.99541131874709055</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.99545545234875521</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.99549958986410092</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.99543338505874523</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.99541131874709055</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.99543328382362717</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.99549958986410092</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.99543338505874523</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.99541131874709055</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.99545545234875521</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.99538915120480598</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.99549958986410092</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.99543338505874523</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.99541131874709055</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.99545545234875521</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.99549958986410092</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.99543338505874523</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.99541131874709055</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.99545545234875521</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.99046351740962524</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.99046351740962524</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.99057440674207142</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.99046351740962524</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2934,11 +3192,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="144"/>
-        <c:axId val="81282560"/>
-        <c:axId val="69133440"/>
+        <c:axId val="46226816"/>
+        <c:axId val="46232704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="81282560"/>
+        <c:axId val="46226816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2947,7 +3205,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69133440"/>
+        <c:crossAx val="46232704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2955,7 +3213,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69133440"/>
+        <c:axId val="46232704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2985,7 +3243,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81282560"/>
+        <c:crossAx val="46226816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3012,16 +3270,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>476942</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>186911</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>288043</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>93261</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>532534</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>151158</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>344435</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>68714</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3048,7 +3306,7 @@
       <xdr:rowOff>93807</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>37</xdr:col>
+      <xdr:col>41</xdr:col>
       <xdr:colOff>242454</xdr:colOff>
       <xdr:row>99</xdr:row>
       <xdr:rowOff>30308</xdr:rowOff>
@@ -3362,10 +3620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:AP39"/>
+  <dimension ref="C2:AT39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="AO48" sqref="AO48"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="AC4" sqref="AC4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3380,32 +3638,36 @@
     <col min="16" max="16" width="9.140625" style="6"/>
     <col min="18" max="18" width="12.28515625" style="6" customWidth="1"/>
     <col min="20" max="20" width="11" style="6" customWidth="1"/>
-    <col min="27" max="27" width="12.42578125" customWidth="1"/>
-    <col min="29" max="29" width="12" customWidth="1"/>
-    <col min="31" max="31" width="11" customWidth="1"/>
-    <col min="33" max="33" width="10.42578125" customWidth="1"/>
+    <col min="25" max="25" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="14.140625" customWidth="1"/>
+    <col min="28" max="28" width="12.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.5703125" customWidth="1"/>
+    <col min="31" max="31" width="12.42578125" customWidth="1"/>
+    <col min="33" max="33" width="12" customWidth="1"/>
+    <col min="35" max="35" width="11" customWidth="1"/>
+    <col min="37" max="37" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:42" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:46" x14ac:dyDescent="0.25">
       <c r="H2" t="s">
         <v>51</v>
       </c>
       <c r="P2" t="s">
         <v>53</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AE2" t="s">
         <v>49</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AM2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="3:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AI3" t="s">
+    <row r="3" spans="3:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AM3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="3:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>34</v>
       </c>
@@ -3445,32 +3707,40 @@
       <c r="W4" s="23" t="s">
         <v>47</v>
       </c>
+      <c r="X4" s="26"/>
+      <c r="Y4" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z4" s="6"/>
       <c r="AA4" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE4" t="s">
         <v>42</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AG4" t="s">
         <v>43</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AI4" t="s">
         <v>44</v>
       </c>
-      <c r="AG4" t="s">
+      <c r="AK4" t="s">
         <v>45</v>
       </c>
-      <c r="AJ4" t="s">
+      <c r="AN4" t="s">
         <v>42</v>
       </c>
-      <c r="AL4" t="s">
+      <c r="AP4" t="s">
         <v>43</v>
       </c>
-      <c r="AN4" t="s">
+      <c r="AR4" t="s">
         <v>44</v>
       </c>
-      <c r="AP4" t="s">
+      <c r="AT4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="3:42" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:46" x14ac:dyDescent="0.25">
       <c r="F5" s="2" t="s">
         <v>37</v>
       </c>
@@ -3507,19 +3777,8 @@
       <c r="S5" t="s">
         <v>38</v>
       </c>
-      <c r="AA5" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="AB5" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC5" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="AD5" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="AE5" s="8" t="s">
+      <c r="Z5" s="6"/>
+      <c r="AE5" s="7" t="s">
         <v>46</v>
       </c>
       <c r="AF5" s="8" t="s">
@@ -3528,17 +3787,29 @@
       <c r="AG5" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="AH5" s="9" t="s">
+      <c r="AH5" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="AJ5" t="s">
+      <c r="AI5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ5" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="AL5" t="s">
+      <c r="AK5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="AL5" s="9" t="s">
         <v>38</v>
       </c>
+      <c r="AN5" t="s">
+        <v>38</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="6" spans="3:42" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>0</v>
       </c>
@@ -3611,67 +3882,86 @@
         <f>V6/$E6</f>
         <v>0.9976056931296694</v>
       </c>
-      <c r="X6" s="1"/>
-      <c r="Y6" s="1"/>
-      <c r="Z6" s="1"/>
-      <c r="AA6" s="10">
+      <c r="X6" s="24">
+        <v>45042</v>
+      </c>
+      <c r="Y6" s="25">
+        <f>X6/$E6</f>
+        <v>0.99855898197618997</v>
+      </c>
+      <c r="Z6" s="6">
+        <v>44904</v>
+      </c>
+      <c r="AA6" s="25">
+        <f>Z6/$E6</f>
+        <v>0.99549958986410092</v>
+      </c>
+      <c r="AB6">
+        <v>44920</v>
+      </c>
+      <c r="AC6" s="25">
+        <f>AB6/$E6</f>
+        <v>0.99585430199303882</v>
+      </c>
+      <c r="AD6" s="1"/>
+      <c r="AE6" s="10">
         <v>41178</v>
-      </c>
-      <c r="AB6" s="11">
-        <f>AA6/$E6</f>
-        <v>0.91289600283769701</v>
-      </c>
-      <c r="AC6" s="12">
-        <v>40042</v>
-      </c>
-      <c r="AD6" s="11">
-        <f>AC6/$E6</f>
-        <v>0.887711441683109</v>
-      </c>
-      <c r="AE6" s="12">
-        <v>40104</v>
       </c>
       <c r="AF6" s="11">
         <f>AE6/$E6</f>
+        <v>0.91289600283769701</v>
+      </c>
+      <c r="AG6" s="12">
+        <v>40042</v>
+      </c>
+      <c r="AH6" s="11">
+        <f>AG6/$E6</f>
+        <v>0.887711441683109</v>
+      </c>
+      <c r="AI6" s="12">
+        <v>40104</v>
+      </c>
+      <c r="AJ6" s="11">
+        <f>AI6/$E6</f>
         <v>0.88908595118274325</v>
       </c>
-      <c r="AG6" s="12">
+      <c r="AK6" s="12">
         <v>39986</v>
       </c>
-      <c r="AH6" s="13">
-        <f>AG6/$E6</f>
+      <c r="AL6" s="13">
+        <f>AK6/$E6</f>
         <v>0.88646994923182654</v>
       </c>
-      <c r="AI6">
+      <c r="AM6">
         <v>31032</v>
-      </c>
-      <c r="AJ6" s="1">
-        <f>AI6/$E6</f>
-        <v>0.68796417407497723</v>
-      </c>
-      <c r="AK6">
-        <v>31507</v>
-      </c>
-      <c r="AL6" s="1">
-        <f>AK6/$E6</f>
-        <v>0.69849469040281997</v>
-      </c>
-      <c r="AM6">
-        <v>30882</v>
       </c>
       <c r="AN6" s="1">
         <f>AM6/$E6</f>
-        <v>0.68463874786618484</v>
+        <v>0.68796417407497723</v>
       </c>
       <c r="AO6">
-        <v>31010</v>
+        <v>31507</v>
       </c>
       <c r="AP6" s="1">
         <f>AO6/$E6</f>
+        <v>0.69849469040281997</v>
+      </c>
+      <c r="AQ6">
+        <v>30882</v>
+      </c>
+      <c r="AR6" s="1">
+        <f>AQ6/$E6</f>
+        <v>0.68463874786618484</v>
+      </c>
+      <c r="AS6">
+        <v>31010</v>
+      </c>
+      <c r="AT6" s="1">
+        <f>AS6/$E6</f>
         <v>0.68747644489768767</v>
       </c>
     </row>
-    <row r="7" spans="3:42" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>1</v>
       </c>
@@ -3744,67 +4034,86 @@
         <f t="shared" ref="W7" si="5">V7/$E7</f>
         <v>0.99521181086652921</v>
       </c>
-      <c r="X7" s="1"/>
-      <c r="Y7" s="1"/>
-      <c r="Z7" s="1"/>
-      <c r="AA7" s="10">
+      <c r="X7" s="24">
+        <v>43518</v>
+      </c>
+      <c r="Y7" s="25">
+        <f>X7/$E7</f>
+        <v>0.96468710514065303</v>
+      </c>
+      <c r="Z7" s="6">
+        <v>44904</v>
+      </c>
+      <c r="AA7" s="25">
+        <f>Z7/$E7</f>
+        <v>0.99541131874709055</v>
+      </c>
+      <c r="AB7">
+        <v>44920</v>
+      </c>
+      <c r="AC7" s="25">
+        <f>AB7/$E7</f>
+        <v>0.99576599942364385</v>
+      </c>
+      <c r="AD7" s="1"/>
+      <c r="AE7" s="10">
         <v>38738</v>
       </c>
-      <c r="AB7" s="11">
-        <f t="shared" ref="AB7:AB39" si="6">AA7/$E7</f>
+      <c r="AF7" s="11">
+        <f t="shared" ref="AF7:AF39" si="6">AE7/$E7</f>
         <v>0.85872625302032768</v>
       </c>
-      <c r="AC7" s="12">
+      <c r="AG7" s="12">
         <v>38598</v>
       </c>
-      <c r="AD7" s="11">
-        <f t="shared" ref="AD7:AD39" si="7">AC7/$E7</f>
+      <c r="AH7" s="11">
+        <f t="shared" ref="AH7:AH39" si="7">AG7/$E7</f>
         <v>0.8556227971004855</v>
       </c>
-      <c r="AE7" s="12">
+      <c r="AI7" s="12">
         <v>37962</v>
       </c>
-      <c r="AF7" s="11">
-        <f t="shared" ref="AF7:AF39" si="8">AE7/$E7</f>
+      <c r="AJ7" s="11">
+        <f t="shared" ref="AJ7:AJ39" si="8">AI7/$E7</f>
         <v>0.84152424020748817</v>
       </c>
-      <c r="AG7" s="12">
+      <c r="AK7" s="12">
         <v>38390</v>
       </c>
-      <c r="AH7" s="13">
-        <f t="shared" ref="AH7:AH39" si="9">AG7/$E7</f>
+      <c r="AL7" s="13">
+        <f t="shared" ref="AL7:AL39" si="9">AK7/$E7</f>
         <v>0.85101194830529137</v>
       </c>
-      <c r="AI7">
+      <c r="AM7">
         <v>32931</v>
       </c>
-      <c r="AJ7" s="1">
-        <f t="shared" ref="AJ7:AL7" si="10">AI7/$E7</f>
+      <c r="AN7" s="1">
+        <f t="shared" ref="AN7:AP7" si="10">AM7/$E7</f>
         <v>0.72999933497373148</v>
       </c>
-      <c r="AK7">
+      <c r="AO7">
         <v>32760</v>
       </c>
-      <c r="AL7" s="1">
+      <c r="AP7" s="1">
         <f t="shared" si="10"/>
         <v>0.72620868524306714</v>
       </c>
-      <c r="AM7">
+      <c r="AQ7">
         <v>33179</v>
       </c>
-      <c r="AN7" s="1">
-        <f t="shared" ref="AN7:AP7" si="11">AM7/$E7</f>
+      <c r="AR7" s="1">
+        <f t="shared" ref="AR7:AT7" si="11">AQ7/$E7</f>
         <v>0.735496885460309</v>
       </c>
-      <c r="AO7">
+      <c r="AS7">
         <v>33294</v>
       </c>
-      <c r="AP7" s="1">
+      <c r="AT7" s="1">
         <f t="shared" si="11"/>
         <v>0.73804615282303654</v>
       </c>
     </row>
-    <row r="8" spans="3:42" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>2</v>
       </c>
@@ -3877,67 +4186,86 @@
         <f t="shared" ref="W8" si="14">V8/$E8</f>
         <v>0.99758368432720013</v>
       </c>
-      <c r="X8" s="1"/>
-      <c r="Y8" s="1"/>
-      <c r="Z8" s="1"/>
-      <c r="AA8" s="10">
+      <c r="X8" s="24">
+        <v>45064</v>
+      </c>
+      <c r="Y8" s="25">
+        <f>X8/$E8</f>
+        <v>0.99898027045001103</v>
+      </c>
+      <c r="Z8" s="6">
+        <v>44904</v>
+      </c>
+      <c r="AA8" s="25">
+        <f>Z8/$E8</f>
+        <v>0.99543338505874523</v>
+      </c>
+      <c r="AB8">
+        <v>44920</v>
+      </c>
+      <c r="AC8" s="25">
+        <f>AB8/$E8</f>
+        <v>0.99578807359787191</v>
+      </c>
+      <c r="AD8" s="1"/>
+      <c r="AE8" s="10">
         <v>41442</v>
       </c>
-      <c r="AB8" s="11">
+      <c r="AF8" s="11">
         <f t="shared" si="6"/>
         <v>0.91868765240523165</v>
       </c>
-      <c r="AC8" s="12">
+      <c r="AG8" s="12">
         <v>40380</v>
       </c>
-      <c r="AD8" s="11">
+      <c r="AH8" s="11">
         <f t="shared" si="7"/>
         <v>0.89514520062070491</v>
       </c>
-      <c r="AE8" s="12">
+      <c r="AI8" s="12">
         <v>40229</v>
       </c>
-      <c r="AF8" s="11">
+      <c r="AJ8" s="11">
         <f t="shared" si="8"/>
         <v>0.89179782753269787</v>
       </c>
-      <c r="AG8" s="12">
+      <c r="AK8" s="12">
         <v>40119</v>
       </c>
-      <c r="AH8" s="13">
+      <c r="AL8" s="13">
         <f t="shared" si="9"/>
         <v>0.88935934382620263</v>
       </c>
-      <c r="AI8">
+      <c r="AM8">
         <v>31241</v>
       </c>
-      <c r="AJ8" s="1">
-        <f t="shared" ref="AJ8:AL8" si="15">AI8/$E8</f>
+      <c r="AN8" s="1">
+        <f t="shared" ref="AN8:AP8" si="15">AM8/$E8</f>
         <v>0.69255154067834179</v>
       </c>
-      <c r="AK8">
+      <c r="AO8">
         <v>30754</v>
       </c>
-      <c r="AL8" s="1">
+      <c r="AP8" s="1">
         <f t="shared" si="15"/>
         <v>0.6817557082686766</v>
       </c>
-      <c r="AM8">
+      <c r="AQ8">
         <v>30896</v>
       </c>
-      <c r="AN8" s="1">
-        <f t="shared" ref="AN8:AP8" si="16">AM8/$E8</f>
+      <c r="AR8" s="1">
+        <f t="shared" ref="AR8:AT8" si="16">AQ8/$E8</f>
         <v>0.68490356905342498</v>
       </c>
-      <c r="AO8">
+      <c r="AS8">
         <v>31261</v>
       </c>
-      <c r="AP8" s="1">
+      <c r="AT8" s="1">
         <f t="shared" si="16"/>
         <v>0.69299490135225006</v>
       </c>
     </row>
-    <row r="9" spans="3:42" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>3</v>
       </c>
@@ -4010,67 +4338,86 @@
         <f t="shared" ref="W9" si="19">V9/$E9</f>
         <v>0.99594333976192062</v>
       </c>
-      <c r="X9" s="1"/>
-      <c r="Y9" s="1"/>
-      <c r="Z9" s="1"/>
-      <c r="AA9" s="10">
+      <c r="X9" s="24">
+        <v>43489</v>
+      </c>
+      <c r="Y9" s="25">
+        <f>X9/$E9</f>
+        <v>0.96404424641440001</v>
+      </c>
+      <c r="Z9" s="6">
+        <v>44904</v>
+      </c>
+      <c r="AA9" s="25">
+        <f>Z9/$E9</f>
+        <v>0.99541131874709055</v>
+      </c>
+      <c r="AB9">
+        <v>44920</v>
+      </c>
+      <c r="AC9" s="25">
+        <f>AB9/$E9</f>
+        <v>0.99576599942364385</v>
+      </c>
+      <c r="AD9" s="1"/>
+      <c r="AE9" s="10">
         <v>41887</v>
       </c>
-      <c r="AB9" s="11">
+      <c r="AF9" s="11">
         <f t="shared" si="6"/>
         <v>0.92853184367449182</v>
       </c>
-      <c r="AC9" s="12">
+      <c r="AG9" s="12">
         <v>41006</v>
       </c>
-      <c r="AD9" s="11">
+      <c r="AH9" s="11">
         <f t="shared" si="7"/>
         <v>0.90900223892177079</v>
       </c>
-      <c r="AE9" s="12">
+      <c r="AI9" s="12">
         <v>40776</v>
       </c>
-      <c r="AF9" s="11">
+      <c r="AJ9" s="11">
         <f t="shared" si="8"/>
         <v>0.90390370419631572</v>
       </c>
-      <c r="AG9" s="12">
+      <c r="AK9" s="12">
         <v>40577</v>
       </c>
-      <c r="AH9" s="13">
+      <c r="AL9" s="13">
         <f t="shared" si="9"/>
         <v>0.89949236328168292</v>
       </c>
-      <c r="AI9">
+      <c r="AM9">
         <v>29983</v>
       </c>
-      <c r="AJ9" s="1">
-        <f t="shared" ref="AJ9:AL9" si="20">AI9/$E9</f>
+      <c r="AN9" s="1">
+        <f t="shared" ref="AN9:AP9" si="20">AM9/$E9</f>
         <v>0.66464942031876928</v>
       </c>
-      <c r="AK9">
+      <c r="AO9">
         <v>30059</v>
       </c>
-      <c r="AL9" s="1">
+      <c r="AP9" s="1">
         <f t="shared" si="20"/>
         <v>0.66633415353239789</v>
       </c>
-      <c r="AM9">
+      <c r="AQ9">
         <v>30174</v>
       </c>
-      <c r="AN9" s="1">
-        <f t="shared" ref="AN9:AP9" si="21">AM9/$E9</f>
+      <c r="AR9" s="1">
+        <f t="shared" ref="AR9:AT9" si="21">AQ9/$E9</f>
         <v>0.66888342089512531</v>
       </c>
-      <c r="AO9">
+      <c r="AS9">
         <v>29797</v>
       </c>
-      <c r="AP9" s="1">
+      <c r="AT9" s="1">
         <f t="shared" si="21"/>
         <v>0.66052625745383609</v>
       </c>
     </row>
-    <row r="10" spans="3:42" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>4</v>
       </c>
@@ -4143,67 +4490,86 @@
         <f t="shared" ref="W10" si="24">V10/$E10</f>
         <v>0.99758373789097998</v>
       </c>
-      <c r="X10" s="1"/>
-      <c r="Y10" s="1"/>
-      <c r="Z10" s="1"/>
-      <c r="AA10" s="10">
+      <c r="X10" s="24">
+        <v>45070</v>
+      </c>
+      <c r="Y10" s="25">
+        <f>X10/$E10</f>
+        <v>0.99909113076633194</v>
+      </c>
+      <c r="Z10" s="6">
+        <v>44904</v>
+      </c>
+      <c r="AA10" s="25">
+        <f>Z10/$E10</f>
+        <v>0.99541131874709055</v>
+      </c>
+      <c r="AB10">
+        <v>44920</v>
+      </c>
+      <c r="AC10" s="25">
+        <f>AB10/$E10</f>
+        <v>0.99576599942364385</v>
+      </c>
+      <c r="AD10" s="1"/>
+      <c r="AE10" s="10">
         <v>40011</v>
       </c>
-      <c r="AB10" s="11">
+      <c r="AF10" s="11">
         <f t="shared" si="6"/>
         <v>0.88694553434860679</v>
       </c>
-      <c r="AC10" s="12">
+      <c r="AG10" s="12">
         <v>38911</v>
       </c>
-      <c r="AD10" s="11">
+      <c r="AH10" s="11">
         <f t="shared" si="7"/>
         <v>0.86256123783556116</v>
       </c>
-      <c r="AE10" s="12">
+      <c r="AI10" s="12">
         <v>39544</v>
       </c>
-      <c r="AF10" s="11">
+      <c r="AJ10" s="11">
         <f t="shared" si="8"/>
         <v>0.87659329210170467</v>
       </c>
-      <c r="AG10" s="12">
+      <c r="AK10" s="12">
         <v>38847</v>
       </c>
-      <c r="AH10" s="13">
+      <c r="AL10" s="13">
         <f t="shared" si="9"/>
         <v>0.86114251512934759</v>
       </c>
-      <c r="AI10">
+      <c r="AM10">
         <v>30494</v>
       </c>
-      <c r="AJ10" s="1">
-        <f t="shared" ref="AJ10:AL10" si="25">AI10/$E10</f>
+      <c r="AN10" s="1">
+        <f t="shared" ref="AN10:AP10" si="25">AM10/$E10</f>
         <v>0.67597703442619317</v>
       </c>
-      <c r="AK10">
+      <c r="AO10">
         <v>30548</v>
       </c>
-      <c r="AL10" s="1">
+      <c r="AP10" s="1">
         <f t="shared" si="25"/>
         <v>0.67717408170956084</v>
       </c>
-      <c r="AM10">
+      <c r="AQ10">
         <v>30856</v>
       </c>
-      <c r="AN10" s="1">
-        <f t="shared" ref="AN10:AP10" si="26">AM10/$E10</f>
+      <c r="AR10" s="1">
+        <f t="shared" ref="AR10:AT10" si="26">AQ10/$E10</f>
         <v>0.68400168473321366</v>
       </c>
-      <c r="AO10">
+      <c r="AS10">
         <v>31068</v>
       </c>
-      <c r="AP10" s="1">
+      <c r="AT10" s="1">
         <f t="shared" si="26"/>
         <v>0.68870120369754606</v>
       </c>
     </row>
-    <row r="11" spans="3:42" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>5</v>
       </c>
@@ -4276,67 +4642,86 @@
         <f t="shared" ref="W11" si="29">V11/$E11</f>
         <v>0.99567732925450558</v>
       </c>
-      <c r="X11" s="1"/>
-      <c r="Y11" s="1"/>
-      <c r="Z11" s="1"/>
-      <c r="AA11" s="10">
+      <c r="X11" s="24">
+        <v>43488</v>
+      </c>
+      <c r="Y11" s="25">
+        <f>X11/$E11</f>
+        <v>0.96402207887211544</v>
+      </c>
+      <c r="Z11" s="6">
+        <v>44904</v>
+      </c>
+      <c r="AA11" s="25">
+        <f>Z11/$E11</f>
+        <v>0.99541131874709055</v>
+      </c>
+      <c r="AB11">
+        <v>44920</v>
+      </c>
+      <c r="AC11" s="25">
+        <f>AB11/$E11</f>
+        <v>0.99576599942364385</v>
+      </c>
+      <c r="AD11" s="1"/>
+      <c r="AE11" s="10">
         <v>37954</v>
       </c>
-      <c r="AB11" s="11">
+      <c r="AF11" s="11">
         <f t="shared" si="6"/>
         <v>0.84134689986921152</v>
       </c>
-      <c r="AC11" s="12">
+      <c r="AG11" s="12">
         <v>37060</v>
       </c>
-      <c r="AD11" s="11">
+      <c r="AH11" s="11">
         <f t="shared" si="7"/>
         <v>0.82152911706679077</v>
       </c>
-      <c r="AE11" s="12">
+      <c r="AI11" s="12">
         <v>37413</v>
       </c>
-      <c r="AF11" s="11">
+      <c r="AJ11" s="11">
         <f t="shared" si="8"/>
         <v>0.82935425949325003</v>
       </c>
-      <c r="AG11" s="12">
+      <c r="AK11" s="12">
         <v>37426</v>
       </c>
-      <c r="AH11" s="13">
+      <c r="AL11" s="13">
         <f t="shared" si="9"/>
         <v>0.82964243754294964</v>
       </c>
-      <c r="AI11">
+      <c r="AM11">
         <v>29392</v>
       </c>
-      <c r="AJ11" s="1">
-        <f t="shared" ref="AJ11:AL11" si="30">AI11/$E11</f>
+      <c r="AN11" s="1">
+        <f t="shared" ref="AN11:AP11" si="30">AM11/$E11</f>
         <v>0.6515484028285784</v>
       </c>
-      <c r="AK11">
+      <c r="AO11">
         <v>28820</v>
       </c>
-      <c r="AL11" s="1">
+      <c r="AP11" s="1">
         <f t="shared" si="30"/>
         <v>0.63886856864179464</v>
       </c>
-      <c r="AM11">
+      <c r="AQ11">
         <v>28635</v>
       </c>
-      <c r="AN11" s="1">
-        <f t="shared" ref="AN11:AP11" si="31">AM11/$E11</f>
+      <c r="AR11" s="1">
+        <f t="shared" ref="AR11:AT11" si="31">AQ11/$E11</f>
         <v>0.63476757331914613</v>
       </c>
-      <c r="AO11">
+      <c r="AS11">
         <v>28670</v>
       </c>
-      <c r="AP11" s="1">
+      <c r="AT11" s="1">
         <f t="shared" si="31"/>
         <v>0.63554343729910667</v>
       </c>
     </row>
-    <row r="12" spans="3:42" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>6</v>
       </c>
@@ -4409,67 +4794,86 @@
         <f t="shared" ref="W12" si="34">V12/$E12</f>
         <v>0.99762796781130147</v>
       </c>
-      <c r="X12" s="1"/>
-      <c r="Y12" s="1"/>
-      <c r="Z12" s="1"/>
-      <c r="AA12" s="10">
+      <c r="X12" s="24">
+        <v>45080</v>
+      </c>
+      <c r="Y12" s="25">
+        <f>X12/$E12</f>
+        <v>0.99935711277128736</v>
+      </c>
+      <c r="Z12" s="6">
+        <v>44904</v>
+      </c>
+      <c r="AA12" s="25">
+        <f>Z12/$E12</f>
+        <v>0.99545545234875521</v>
+      </c>
+      <c r="AB12">
+        <v>44920</v>
+      </c>
+      <c r="AC12" s="25">
+        <f>AB12/$E12</f>
+        <v>0.99581014875080365</v>
+      </c>
+      <c r="AD12" s="1"/>
+      <c r="AE12" s="10">
         <v>38653</v>
       </c>
-      <c r="AB12" s="11">
+      <c r="AF12" s="11">
         <f t="shared" si="6"/>
         <v>0.856880001773482</v>
       </c>
-      <c r="AC12" s="12">
+      <c r="AG12" s="12">
         <v>37049</v>
       </c>
-      <c r="AD12" s="11">
+      <c r="AH12" s="11">
         <f t="shared" si="7"/>
         <v>0.82132168746813272</v>
       </c>
-      <c r="AE12" s="12">
+      <c r="AI12" s="12">
         <v>37054</v>
       </c>
-      <c r="AF12" s="11">
+      <c r="AJ12" s="11">
         <f t="shared" si="8"/>
         <v>0.82143253009377282</v>
       </c>
-      <c r="AG12" s="12">
+      <c r="AK12" s="12">
         <v>37317</v>
       </c>
-      <c r="AH12" s="13">
+      <c r="AL12" s="13">
         <f t="shared" si="9"/>
         <v>0.827262852202443</v>
       </c>
-      <c r="AI12">
+      <c r="AM12">
         <v>30006</v>
       </c>
-      <c r="AJ12" s="1">
-        <f t="shared" ref="AJ12:AL12" si="35">AI12/$E12</f>
+      <c r="AN12" s="1">
+        <f t="shared" ref="AN12:AP12" si="35">AM12/$E12</f>
         <v>0.66518876499146506</v>
       </c>
-      <c r="AK12">
+      <c r="AO12">
         <v>30011</v>
       </c>
-      <c r="AL12" s="1">
+      <c r="AP12" s="1">
         <f t="shared" si="35"/>
         <v>0.66529960761710527</v>
       </c>
-      <c r="AM12">
+      <c r="AQ12">
         <v>30275</v>
       </c>
-      <c r="AN12" s="1">
-        <f t="shared" ref="AN12:AP12" si="36">AM12/$E12</f>
+      <c r="AR12" s="1">
+        <f t="shared" ref="AR12:AT12" si="36">AQ12/$E12</f>
         <v>0.67115209825090338</v>
       </c>
-      <c r="AO12">
+      <c r="AS12">
         <v>29956</v>
       </c>
-      <c r="AP12" s="1">
+      <c r="AT12" s="1">
         <f t="shared" si="36"/>
         <v>0.664080338735064</v>
       </c>
     </row>
-    <row r="13" spans="3:42" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>7</v>
       </c>
@@ -4542,67 +4946,86 @@
         <f t="shared" ref="W13" si="39">V13/$E13</f>
         <v>0.99596550730420519</v>
       </c>
-      <c r="X13" s="1"/>
-      <c r="Y13" s="1"/>
-      <c r="Z13" s="1"/>
-      <c r="AA13" s="10">
+      <c r="X13" s="24">
+        <v>43482</v>
+      </c>
+      <c r="Y13" s="25">
+        <f>X13/$E13</f>
+        <v>0.96388907361840792</v>
+      </c>
+      <c r="Z13" s="6">
+        <v>44904</v>
+      </c>
+      <c r="AA13" s="25">
+        <f>Z13/$E13</f>
+        <v>0.99541131874709055</v>
+      </c>
+      <c r="AB13">
+        <v>44920</v>
+      </c>
+      <c r="AC13" s="25">
+        <f>AB13/$E13</f>
+        <v>0.99576599942364385</v>
+      </c>
+      <c r="AD13" s="1"/>
+      <c r="AE13" s="10">
         <v>39273</v>
       </c>
-      <c r="AB13" s="11">
+      <c r="AF13" s="11">
         <f t="shared" si="6"/>
         <v>0.87058588814258164</v>
       </c>
-      <c r="AC13" s="12">
+      <c r="AG13" s="12">
         <v>38167</v>
       </c>
-      <c r="AD13" s="11">
+      <c r="AH13" s="11">
         <f t="shared" si="7"/>
         <v>0.84606858637582849</v>
       </c>
-      <c r="AE13" s="12">
+      <c r="AI13" s="12">
         <v>38391</v>
       </c>
-      <c r="AF13" s="11">
+      <c r="AJ13" s="11">
         <f t="shared" si="8"/>
         <v>0.85103411584757593</v>
       </c>
-      <c r="AG13" s="12">
+      <c r="AK13" s="12">
         <v>38145</v>
       </c>
-      <c r="AH13" s="13">
+      <c r="AL13" s="13">
         <f t="shared" si="9"/>
         <v>0.84558090044556755</v>
       </c>
-      <c r="AI13">
+      <c r="AM13">
         <v>27462</v>
       </c>
-      <c r="AJ13" s="1">
-        <f t="shared" ref="AJ13:AL13" si="40">AI13/$E13</f>
+      <c r="AN13" s="1">
+        <f t="shared" ref="AN13:AP13" si="40">AM13/$E13</f>
         <v>0.6087650462193257</v>
       </c>
-      <c r="AK13">
+      <c r="AO13">
         <v>27381</v>
       </c>
-      <c r="AL13" s="1">
+      <c r="AP13" s="1">
         <f t="shared" si="40"/>
         <v>0.60696947529427414</v>
       </c>
-      <c r="AM13">
+      <c r="AQ13">
         <v>27585</v>
       </c>
-      <c r="AN13" s="1">
-        <f t="shared" ref="AN13:AP13" si="41">AM13/$E13</f>
+      <c r="AR13" s="1">
+        <f t="shared" ref="AR13:AT13" si="41">AQ13/$E13</f>
         <v>0.61149165392032989</v>
       </c>
-      <c r="AO13">
+      <c r="AS13">
         <v>27901</v>
       </c>
-      <c r="AP13" s="1">
+      <c r="AT13" s="1">
         <f t="shared" si="41"/>
         <v>0.61849659728225936</v>
       </c>
     </row>
-    <row r="14" spans="3:42" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C14">
         <v>8</v>
       </c>
@@ -4675,67 +5098,86 @@
         <f t="shared" ref="W14" si="44">V14/$E14</f>
         <v>0.99769437116190396</v>
       </c>
-      <c r="X14" s="1"/>
-      <c r="Y14" s="1"/>
-      <c r="Z14" s="1"/>
-      <c r="AA14" s="10">
+      <c r="X14" s="24">
+        <v>45067</v>
+      </c>
+      <c r="Y14" s="25">
+        <f>X14/$E14</f>
+        <v>0.99911321967765532</v>
+      </c>
+      <c r="Z14" s="6">
+        <v>44904</v>
+      </c>
+      <c r="AA14" s="25">
+        <f>Z14/$E14</f>
+        <v>0.99549958986410092</v>
+      </c>
+      <c r="AB14">
+        <v>44920</v>
+      </c>
+      <c r="AC14" s="25">
+        <f>AB14/$E14</f>
+        <v>0.99585430199303882</v>
+      </c>
+      <c r="AD14" s="1"/>
+      <c r="AE14" s="10">
         <v>38858</v>
       </c>
-      <c r="AB14" s="11">
+      <c r="AF14" s="11">
         <f t="shared" si="6"/>
         <v>0.86146274414170754</v>
       </c>
-      <c r="AC14" s="12">
+      <c r="AG14" s="12">
         <v>38045</v>
       </c>
-      <c r="AD14" s="11">
+      <c r="AH14" s="11">
         <f t="shared" si="7"/>
         <v>0.84343893409005255</v>
       </c>
-      <c r="AE14" s="12">
+      <c r="AI14" s="12">
         <v>38412</v>
       </c>
-      <c r="AF14" s="11">
+      <c r="AJ14" s="11">
         <f t="shared" si="8"/>
         <v>0.85157514354756469</v>
       </c>
-      <c r="AG14" s="12">
+      <c r="AK14" s="12">
         <v>37880</v>
       </c>
-      <c r="AH14" s="13">
+      <c r="AL14" s="13">
         <f t="shared" si="9"/>
         <v>0.83978096526038082</v>
       </c>
-      <c r="AI14">
+      <c r="AM14">
         <v>27535</v>
       </c>
-      <c r="AJ14" s="1">
-        <f t="shared" ref="AJ14:AL14" si="45">AI14/$E14</f>
+      <c r="AN14" s="1">
+        <f t="shared" ref="AN14:AP14" si="45">AM14/$E14</f>
         <v>0.61043740439399652</v>
       </c>
-      <c r="AK14">
+      <c r="AO14">
         <v>27307</v>
       </c>
-      <c r="AL14" s="1">
+      <c r="AP14" s="1">
         <f t="shared" si="45"/>
         <v>0.60538275655663198</v>
       </c>
-      <c r="AM14">
+      <c r="AQ14">
         <v>27291</v>
       </c>
-      <c r="AN14" s="1">
-        <f t="shared" ref="AN14:AP14" si="46">AM14/$E14</f>
+      <c r="AR14" s="1">
+        <f t="shared" ref="AR14:AT14" si="46">AQ14/$E14</f>
         <v>0.6050280444276942</v>
       </c>
-      <c r="AO14">
+      <c r="AS14">
         <v>27347</v>
       </c>
-      <c r="AP14" s="1">
+      <c r="AT14" s="1">
         <f t="shared" si="46"/>
         <v>0.60626953687897667</v>
       </c>
     </row>
-    <row r="15" spans="3:42" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C15">
         <v>9</v>
       </c>
@@ -4808,67 +5250,86 @@
         <f t="shared" ref="W15" si="49">V15/$E15</f>
         <v>0.99758368432720013</v>
       </c>
-      <c r="X15" s="1"/>
-      <c r="Y15" s="1"/>
-      <c r="Z15" s="1"/>
-      <c r="AA15" s="10">
+      <c r="X15" s="24">
+        <v>45084</v>
+      </c>
+      <c r="Y15" s="25">
+        <f>X15/$E15</f>
+        <v>0.9994236311239193</v>
+      </c>
+      <c r="Z15" s="6">
+        <v>44904</v>
+      </c>
+      <c r="AA15" s="25">
+        <f>Z15/$E15</f>
+        <v>0.99543338505874523</v>
+      </c>
+      <c r="AB15">
+        <v>44920</v>
+      </c>
+      <c r="AC15" s="25">
+        <f>AB15/$E15</f>
+        <v>0.99578807359787191</v>
+      </c>
+      <c r="AD15" s="1"/>
+      <c r="AE15" s="10">
         <v>41574</v>
       </c>
-      <c r="AB15" s="11">
+      <c r="AF15" s="11">
         <f t="shared" si="6"/>
         <v>0.92161383285302589</v>
       </c>
-      <c r="AC15" s="12">
+      <c r="AG15" s="12">
         <v>40486</v>
       </c>
-      <c r="AD15" s="11">
+      <c r="AH15" s="11">
         <f t="shared" si="7"/>
         <v>0.89749501219241856</v>
       </c>
-      <c r="AE15" s="12">
+      <c r="AI15" s="12">
         <v>40345</v>
       </c>
-      <c r="AF15" s="11">
+      <c r="AJ15" s="11">
         <f t="shared" si="8"/>
         <v>0.89436931944136555</v>
       </c>
-      <c r="AG15" s="12">
+      <c r="AK15" s="12">
         <v>40342</v>
       </c>
-      <c r="AH15" s="13">
+      <c r="AL15" s="13">
         <f t="shared" si="9"/>
         <v>0.89430281534027933</v>
       </c>
-      <c r="AI15">
+      <c r="AM15">
         <v>27488</v>
       </c>
-      <c r="AJ15" s="1">
-        <f t="shared" ref="AJ15:AL15" si="50">AI15/$E15</f>
+      <c r="AN15" s="1">
+        <f t="shared" ref="AN15:AP15" si="50">AM15/$E15</f>
         <v>0.60935491021946353</v>
       </c>
-      <c r="AK15">
+      <c r="AO15">
         <v>26963</v>
       </c>
-      <c r="AL15" s="1">
+      <c r="AP15" s="1">
         <f t="shared" si="50"/>
         <v>0.59771669252937265</v>
       </c>
-      <c r="AM15">
+      <c r="AQ15">
         <v>26816</v>
       </c>
-      <c r="AN15" s="1">
-        <f t="shared" ref="AN15:AP15" si="51">AM15/$E15</f>
+      <c r="AR15" s="1">
+        <f t="shared" ref="AR15:AT15" si="51">AQ15/$E15</f>
         <v>0.5944579915761472</v>
       </c>
-      <c r="AO15">
+      <c r="AS15">
         <v>26540</v>
       </c>
-      <c r="AP15" s="1">
+      <c r="AT15" s="1">
         <f t="shared" si="51"/>
         <v>0.58833961427621373</v>
       </c>
     </row>
-    <row r="16" spans="3:42" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C16">
         <v>10</v>
       </c>
@@ -4941,67 +5402,86 @@
         <f t="shared" ref="W16" si="54">V16/$E16</f>
         <v>0.99745073263727246</v>
       </c>
-      <c r="X16" s="1"/>
-      <c r="Y16" s="1"/>
-      <c r="Z16" s="1"/>
-      <c r="AA16" s="10">
+      <c r="X16" s="24">
+        <v>45082</v>
+      </c>
+      <c r="Y16" s="25">
+        <f>X16/$E16</f>
+        <v>0.99935714127374697</v>
+      </c>
+      <c r="Z16" s="6">
+        <v>44904</v>
+      </c>
+      <c r="AA16" s="25">
+        <f>Z16/$E16</f>
+        <v>0.99541131874709055</v>
+      </c>
+      <c r="AB16">
+        <v>44920</v>
+      </c>
+      <c r="AC16" s="25">
+        <f>AB16/$E16</f>
+        <v>0.99576599942364385</v>
+      </c>
+      <c r="AD16" s="1"/>
+      <c r="AE16" s="10">
         <v>41078</v>
       </c>
-      <c r="AB16" s="11">
+      <c r="AF16" s="11">
         <f t="shared" si="6"/>
         <v>0.91059830196626101</v>
       </c>
-      <c r="AC16" s="12">
+      <c r="AG16" s="12">
         <v>40075</v>
       </c>
-      <c r="AD16" s="11">
+      <c r="AH16" s="11">
         <f t="shared" si="7"/>
         <v>0.88836425705482036</v>
       </c>
-      <c r="AE16" s="12">
+      <c r="AI16" s="12">
         <v>39746</v>
       </c>
-      <c r="AF16" s="11">
+      <c r="AJ16" s="11">
         <f t="shared" si="8"/>
         <v>0.88107113564319128</v>
       </c>
-      <c r="AG16" s="12">
+      <c r="AK16" s="12">
         <v>40126</v>
       </c>
-      <c r="AH16" s="13">
+      <c r="AL16" s="13">
         <f t="shared" si="9"/>
         <v>0.88949480171133422</v>
       </c>
-      <c r="AI16">
+      <c r="AM16">
         <v>26190</v>
       </c>
-      <c r="AJ16" s="1">
-        <f t="shared" ref="AJ16:AL16" si="55">AI16/$E16</f>
+      <c r="AN16" s="1">
+        <f t="shared" ref="AN16:AP16" si="55">AM16/$E16</f>
         <v>0.58056793243333116</v>
       </c>
-      <c r="AK16">
+      <c r="AO16">
         <v>26839</v>
       </c>
-      <c r="AL16" s="1">
+      <c r="AP16" s="1">
         <f t="shared" si="55"/>
         <v>0.59495466737602798</v>
       </c>
-      <c r="AM16">
+      <c r="AQ16">
         <v>27180</v>
       </c>
-      <c r="AN16" s="1">
-        <f t="shared" ref="AN16:AP16" si="56">AM16/$E16</f>
+      <c r="AR16" s="1">
+        <f t="shared" ref="AR16:AT16" si="56">AQ16/$E16</f>
         <v>0.60251379929507221</v>
       </c>
-      <c r="AO16">
+      <c r="AS16">
         <v>26494</v>
       </c>
-      <c r="AP16" s="1">
+      <c r="AT16" s="1">
         <f t="shared" si="56"/>
         <v>0.58730686528784559</v>
       </c>
     </row>
-    <row r="17" spans="3:42" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C17">
         <v>11</v>
       </c>
@@ -5074,67 +5554,86 @@
         <f t="shared" ref="W17" si="59">V17/$E17</f>
         <v>0.99760579928617354</v>
       </c>
-      <c r="X17" s="1"/>
-      <c r="Y17" s="1"/>
-      <c r="Z17" s="1"/>
-      <c r="AA17" s="10">
+      <c r="X17" s="24">
+        <v>45088</v>
+      </c>
+      <c r="Y17" s="25">
+        <f>X17/$E17</f>
+        <v>0.99953446097231147</v>
+      </c>
+      <c r="Z17" s="6">
+        <v>44904</v>
+      </c>
+      <c r="AA17" s="25">
+        <f>Z17/$E17</f>
+        <v>0.99545545234875521</v>
+      </c>
+      <c r="AB17">
+        <v>44920</v>
+      </c>
+      <c r="AC17" s="25">
+        <f>AB17/$E17</f>
+        <v>0.99581014875080365</v>
+      </c>
+      <c r="AD17" s="1"/>
+      <c r="AE17" s="10">
         <v>40332</v>
       </c>
-      <c r="AB17" s="11">
+      <c r="AF17" s="11">
         <f t="shared" si="6"/>
         <v>0.89410095546343304</v>
       </c>
-      <c r="AC17" s="12">
+      <c r="AG17" s="12">
         <v>39448</v>
       </c>
-      <c r="AD17" s="11">
+      <c r="AH17" s="11">
         <f t="shared" si="7"/>
         <v>0.87450397925026047</v>
       </c>
-      <c r="AE17" s="12">
+      <c r="AI17" s="12">
         <v>39313</v>
       </c>
-      <c r="AF17" s="11">
+      <c r="AJ17" s="11">
         <f t="shared" si="8"/>
         <v>0.87151122835797734</v>
       </c>
-      <c r="AG17" s="12">
+      <c r="AK17" s="12">
         <v>39707</v>
       </c>
-      <c r="AH17" s="13">
+      <c r="AL17" s="13">
         <f t="shared" si="9"/>
         <v>0.88024562725841848</v>
       </c>
-      <c r="AI17">
+      <c r="AM17">
         <v>25788</v>
       </c>
-      <c r="AJ17" s="1">
-        <f t="shared" ref="AJ17:AL17" si="60">AI17/$E17</f>
+      <c r="AN17" s="1">
+        <f t="shared" ref="AN17:AP17" si="60">AM17/$E17</f>
         <v>0.57168192600146317</v>
       </c>
-      <c r="AK17">
+      <c r="AO17">
         <v>26663</v>
       </c>
-      <c r="AL17" s="1">
+      <c r="AP17" s="1">
         <f t="shared" si="60"/>
         <v>0.59107938548848349</v>
       </c>
-      <c r="AM17">
+      <c r="AQ17">
         <v>26596</v>
       </c>
-      <c r="AN17" s="1">
-        <f t="shared" ref="AN17:AP17" si="61">AM17/$E17</f>
+      <c r="AR17" s="1">
+        <f t="shared" ref="AR17:AT17" si="61">AQ17/$E17</f>
         <v>0.58959409430490595</v>
       </c>
-      <c r="AO17">
+      <c r="AS17">
         <v>26586</v>
       </c>
-      <c r="AP17" s="1">
+      <c r="AT17" s="1">
         <f t="shared" si="61"/>
         <v>0.58937240905362565</v>
       </c>
     </row>
-    <row r="18" spans="3:42" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C18">
         <v>12</v>
       </c>
@@ -5207,67 +5706,86 @@
         <f t="shared" ref="W18" si="64">V18/$E18</f>
         <v>0.99756135411355218</v>
       </c>
-      <c r="X18" s="1"/>
-      <c r="Y18" s="1"/>
-      <c r="Z18" s="1"/>
-      <c r="AA18" s="10">
+      <c r="X18" s="24">
+        <v>45073</v>
+      </c>
+      <c r="Y18" s="25">
+        <f>X18/$E18</f>
+        <v>0.9992462367260071</v>
+      </c>
+      <c r="Z18" s="6">
+        <v>44904</v>
+      </c>
+      <c r="AA18" s="25">
+        <f>Z18/$E18</f>
+        <v>0.99549958986410092</v>
+      </c>
+      <c r="AB18">
+        <v>44920</v>
+      </c>
+      <c r="AC18" s="25">
+        <f>AB18/$E18</f>
+        <v>0.99585430199303882</v>
+      </c>
+      <c r="AD18" s="1"/>
+      <c r="AE18" s="10">
         <v>40749</v>
       </c>
-      <c r="AB18" s="11">
+      <c r="AF18" s="11">
         <f t="shared" si="6"/>
         <v>0.90338528388055073</v>
       </c>
-      <c r="AC18" s="12">
+      <c r="AG18" s="12">
         <v>39843</v>
       </c>
-      <c r="AD18" s="11">
+      <c r="AH18" s="11">
         <f t="shared" si="7"/>
         <v>0.88329970957944448</v>
       </c>
-      <c r="AE18" s="12">
+      <c r="AI18" s="12">
         <v>39579</v>
       </c>
-      <c r="AF18" s="11">
+      <c r="AJ18" s="11">
         <f t="shared" si="8"/>
         <v>0.87744695945196971</v>
       </c>
-      <c r="AG18" s="12">
+      <c r="AK18" s="12">
         <v>39687</v>
       </c>
-      <c r="AH18" s="13">
+      <c r="AL18" s="13">
         <f t="shared" si="9"/>
         <v>0.87984126632230031</v>
       </c>
-      <c r="AI18">
+      <c r="AM18">
         <v>27380</v>
       </c>
-      <c r="AJ18" s="1">
-        <f t="shared" ref="AJ18:AL18" si="65">AI18/$E18</f>
+      <c r="AN18" s="1">
+        <f t="shared" ref="AN18:AP18" si="65">AM18/$E18</f>
         <v>0.60700113064491101</v>
       </c>
-      <c r="AK18">
+      <c r="AO18">
         <v>26232</v>
       </c>
-      <c r="AL18" s="1">
+      <c r="AP18" s="1">
         <f t="shared" si="65"/>
         <v>0.58155053539361956</v>
       </c>
-      <c r="AM18">
+      <c r="AQ18">
         <v>26016</v>
       </c>
-      <c r="AN18" s="1">
-        <f t="shared" ref="AN18:AP18" si="66">AM18/$E18</f>
+      <c r="AR18" s="1">
+        <f t="shared" ref="AR18:AT18" si="66">AQ18/$E18</f>
         <v>0.57676192165295848</v>
       </c>
-      <c r="AO18">
+      <c r="AS18">
         <v>26811</v>
       </c>
-      <c r="AP18" s="1">
+      <c r="AT18" s="1">
         <f t="shared" si="66"/>
         <v>0.59438668055955834</v>
       </c>
     </row>
-    <row r="19" spans="3:42" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C19">
         <v>13</v>
       </c>
@@ -5340,67 +5858,86 @@
         <f t="shared" ref="W19" si="69">V19/$E19</f>
         <v>0.99756151629350476</v>
       </c>
-      <c r="X19" s="1"/>
-      <c r="Y19" s="1"/>
-      <c r="Z19" s="1"/>
-      <c r="AA19" s="10">
+      <c r="X19" s="24">
+        <v>45095</v>
+      </c>
+      <c r="Y19" s="25">
+        <f>X19/$E19</f>
+        <v>0.9996674794945688</v>
+      </c>
+      <c r="Z19" s="6">
+        <v>44904</v>
+      </c>
+      <c r="AA19" s="25">
+        <f>Z19/$E19</f>
+        <v>0.99543338505874523</v>
+      </c>
+      <c r="AB19">
+        <v>44920</v>
+      </c>
+      <c r="AC19" s="25">
+        <f>AB19/$E19</f>
+        <v>0.99578807359787191</v>
+      </c>
+      <c r="AD19" s="1"/>
+      <c r="AE19" s="10">
         <v>41172</v>
       </c>
-      <c r="AB19" s="11">
+      <c r="AF19" s="11">
         <f t="shared" si="6"/>
         <v>0.91270228330747061</v>
       </c>
-      <c r="AC19" s="12">
+      <c r="AG19" s="12">
         <v>40153</v>
       </c>
-      <c r="AD19" s="11">
+      <c r="AH19" s="11">
         <f t="shared" si="7"/>
         <v>0.89011305697184662</v>
       </c>
-      <c r="AE19" s="12">
+      <c r="AI19" s="12">
         <v>39989</v>
       </c>
-      <c r="AF19" s="11">
+      <c r="AJ19" s="11">
         <f t="shared" si="8"/>
         <v>0.88647749944579912</v>
       </c>
-      <c r="AG19" s="12">
+      <c r="AK19" s="12">
         <v>40015</v>
       </c>
-      <c r="AH19" s="13">
+      <c r="AL19" s="13">
         <f t="shared" si="9"/>
         <v>0.88705386832187982</v>
       </c>
-      <c r="AI19">
+      <c r="AM19">
         <v>27437</v>
       </c>
-      <c r="AJ19" s="1">
-        <f t="shared" ref="AJ19:AL19" si="70">AI19/$E19</f>
+      <c r="AN19" s="1">
+        <f t="shared" ref="AN19:AP19" si="70">AM19/$E19</f>
         <v>0.60822434050099761</v>
       </c>
-      <c r="AK19">
+      <c r="AO19">
         <v>26461</v>
       </c>
-      <c r="AL19" s="1">
+      <c r="AP19" s="1">
         <f t="shared" si="70"/>
         <v>0.58658833961427626</v>
       </c>
-      <c r="AM19">
+      <c r="AQ19">
         <v>26712</v>
       </c>
-      <c r="AN19" s="1">
-        <f t="shared" ref="AN19:AP19" si="71">AM19/$E19</f>
+      <c r="AR19" s="1">
+        <f t="shared" ref="AR19:AT19" si="71">AQ19/$E19</f>
         <v>0.5921525160718244</v>
       </c>
-      <c r="AO19">
+      <c r="AS19">
         <v>26111</v>
       </c>
-      <c r="AP19" s="1">
+      <c r="AT19" s="1">
         <f t="shared" si="71"/>
         <v>0.57882952782088226</v>
       </c>
     </row>
-    <row r="20" spans="3:42" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>14</v>
       </c>
@@ -5473,67 +6010,86 @@
         <f t="shared" ref="W20" si="74">V20/$E20</f>
         <v>0.99747290017955714</v>
       </c>
-      <c r="X20" s="1"/>
-      <c r="Y20" s="1"/>
-      <c r="Z20" s="1"/>
-      <c r="AA20" s="10">
+      <c r="X20" s="24">
+        <v>45099</v>
+      </c>
+      <c r="Y20" s="25">
+        <f>X20/$E20</f>
+        <v>0.99973398949258496</v>
+      </c>
+      <c r="Z20" s="6">
+        <v>44904</v>
+      </c>
+      <c r="AA20" s="25">
+        <f>Z20/$E20</f>
+        <v>0.99541131874709055</v>
+      </c>
+      <c r="AB20">
+        <v>44920</v>
+      </c>
+      <c r="AC20" s="25">
+        <f>AB20/$E20</f>
+        <v>0.99576599942364385</v>
+      </c>
+      <c r="AD20" s="1"/>
+      <c r="AE20" s="10">
         <v>41575</v>
       </c>
-      <c r="AB20" s="11">
+      <c r="AF20" s="11">
         <f t="shared" si="6"/>
         <v>0.92161557048170073</v>
       </c>
-      <c r="AC20" s="12">
+      <c r="AG20" s="12">
         <v>40291</v>
       </c>
-      <c r="AD20" s="11">
+      <c r="AH20" s="11">
         <f t="shared" si="7"/>
         <v>0.89315244618829115</v>
       </c>
-      <c r="AE20" s="12">
+      <c r="AI20" s="12">
         <v>40535</v>
       </c>
-      <c r="AF20" s="11">
+      <c r="AJ20" s="11">
         <f t="shared" si="8"/>
         <v>0.89856132650573028</v>
       </c>
-      <c r="AG20" s="12">
+      <c r="AK20" s="12">
         <v>40459</v>
       </c>
-      <c r="AH20" s="13">
+      <c r="AL20" s="13">
         <f t="shared" si="9"/>
         <v>0.89687659329210168</v>
       </c>
-      <c r="AI20">
+      <c r="AM20">
         <v>25912</v>
       </c>
-      <c r="AJ20" s="1">
-        <f t="shared" ref="AJ20:AL20" si="75">AI20/$E20</f>
+      <c r="AN20" s="1">
+        <f t="shared" ref="AN20:AP20" si="75">AM20/$E20</f>
         <v>0.57440535567821593</v>
       </c>
-      <c r="AK20">
+      <c r="AO20">
         <v>26995</v>
       </c>
-      <c r="AL20" s="1">
+      <c r="AP20" s="1">
         <f t="shared" si="75"/>
         <v>0.59841280397242358</v>
       </c>
-      <c r="AM20">
+      <c r="AQ20">
         <v>27172</v>
       </c>
-      <c r="AN20" s="1">
-        <f t="shared" ref="AN20:AP20" si="76">AM20/$E20</f>
+      <c r="AR20" s="1">
+        <f t="shared" ref="AR20:AT20" si="76">AQ20/$E20</f>
         <v>0.60233645895679544</v>
       </c>
-      <c r="AO20">
+      <c r="AS20">
         <v>26704</v>
       </c>
-      <c r="AP20" s="1">
+      <c r="AT20" s="1">
         <f t="shared" si="76"/>
         <v>0.59196204916760875</v>
       </c>
     </row>
-    <row r="21" spans="3:42" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C21">
         <v>15</v>
       </c>
@@ -5606,67 +6162,86 @@
         <f t="shared" ref="W21" si="79">V21/$E21</f>
         <v>0.99751712518566138</v>
       </c>
-      <c r="X21" s="1"/>
-      <c r="Y21" s="1"/>
-      <c r="Z21" s="1"/>
-      <c r="AA21" s="10">
+      <c r="X21" s="24">
+        <v>45032</v>
+      </c>
+      <c r="Y21" s="25">
+        <f>X21/$E21</f>
+        <v>0.99829302356514216</v>
+      </c>
+      <c r="Z21" s="6">
+        <v>44903</v>
+      </c>
+      <c r="AA21" s="25">
+        <f>Z21/$E21</f>
+        <v>0.99543328382362717</v>
+      </c>
+      <c r="AB21">
+        <v>44920</v>
+      </c>
+      <c r="AC21" s="25">
+        <f>AB21/$E21</f>
+        <v>0.99581014875080365</v>
+      </c>
+      <c r="AD21" s="1"/>
+      <c r="AE21" s="10">
         <v>41564</v>
       </c>
-      <c r="AB21" s="11">
+      <c r="AF21" s="11">
         <f t="shared" si="6"/>
         <v>0.92141257842115765</v>
       </c>
-      <c r="AC21" s="12">
+      <c r="AG21" s="12">
         <v>40757</v>
       </c>
-      <c r="AD21" s="11">
+      <c r="AH21" s="11">
         <f t="shared" si="7"/>
         <v>0.90352257864284291</v>
       </c>
-      <c r="AE21" s="12">
+      <c r="AI21" s="12">
         <v>40572</v>
       </c>
-      <c r="AF21" s="11">
+      <c r="AJ21" s="11">
         <f t="shared" si="8"/>
         <v>0.89942140149415861</v>
       </c>
-      <c r="AG21" s="12">
+      <c r="AK21" s="12">
         <v>40534</v>
       </c>
-      <c r="AH21" s="13">
+      <c r="AL21" s="13">
         <f t="shared" si="9"/>
         <v>0.89857899753929371</v>
       </c>
-      <c r="AI21">
+      <c r="AM21">
         <v>25804</v>
       </c>
-      <c r="AJ21" s="1">
-        <f t="shared" ref="AJ21:AL21" si="80">AI21/$E21</f>
+      <c r="AN21" s="1">
+        <f t="shared" ref="AN21:AP21" si="80">AM21/$E21</f>
         <v>0.5720366224035115</v>
       </c>
-      <c r="AK21">
+      <c r="AO21">
         <v>26264</v>
       </c>
-      <c r="AL21" s="1">
+      <c r="AP21" s="1">
         <f t="shared" si="80"/>
         <v>0.58223414396240214</v>
       </c>
-      <c r="AM21">
+      <c r="AQ21">
         <v>26300</v>
       </c>
-      <c r="AN21" s="1">
-        <f t="shared" ref="AN21:AP21" si="81">AM21/$E21</f>
+      <c r="AR21" s="1">
+        <f t="shared" ref="AR21:AT21" si="81">AQ21/$E21</f>
         <v>0.58303221086701107</v>
       </c>
-      <c r="AO21">
+      <c r="AS21">
         <v>26605</v>
       </c>
-      <c r="AP21" s="1">
+      <c r="AT21" s="1">
         <f t="shared" si="81"/>
         <v>0.5897936110310581</v>
       </c>
     </row>
-    <row r="22" spans="3:42" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C22">
         <v>16</v>
       </c>
@@ -5739,67 +6314,86 @@
         <f t="shared" ref="W22" si="84">V22/$E22</f>
         <v>0.99769437116190396</v>
       </c>
-      <c r="X22" s="1"/>
-      <c r="Y22" s="1"/>
-      <c r="Z22" s="1"/>
-      <c r="AA22" s="10">
+      <c r="X22" s="24">
+        <v>45092</v>
+      </c>
+      <c r="Y22" s="25">
+        <f>X22/$E22</f>
+        <v>0.99966745737912077</v>
+      </c>
+      <c r="Z22" s="6">
+        <v>44904</v>
+      </c>
+      <c r="AA22" s="25">
+        <f>Z22/$E22</f>
+        <v>0.99549958986410092</v>
+      </c>
+      <c r="AB22">
+        <v>44920</v>
+      </c>
+      <c r="AC22" s="25">
+        <f>AB22/$E22</f>
+        <v>0.99585430199303882</v>
+      </c>
+      <c r="AD22" s="1"/>
+      <c r="AE22" s="10">
         <v>39491</v>
       </c>
-      <c r="AB22" s="11">
+      <c r="AF22" s="11">
         <f t="shared" si="6"/>
         <v>0.87549604274281156</v>
       </c>
-      <c r="AC22" s="12">
+      <c r="AG22" s="12">
         <v>38626</v>
       </c>
-      <c r="AD22" s="11">
+      <c r="AH22" s="11">
         <f t="shared" si="7"/>
         <v>0.85631941827210856</v>
       </c>
-      <c r="AE22" s="12">
+      <c r="AI22" s="12">
         <v>38820</v>
       </c>
-      <c r="AF22" s="11">
+      <c r="AJ22" s="11">
         <f t="shared" si="8"/>
         <v>0.86062030283548008</v>
       </c>
-      <c r="AG22" s="12">
+      <c r="AK22" s="12">
         <v>38579</v>
       </c>
-      <c r="AH22" s="13">
+      <c r="AL22" s="13">
         <f t="shared" si="9"/>
         <v>0.85527745139335354</v>
       </c>
-      <c r="AI22">
+      <c r="AM22">
         <v>27499</v>
       </c>
-      <c r="AJ22" s="1">
-        <f t="shared" ref="AJ22:AL22" si="85">AI22/$E22</f>
+      <c r="AN22" s="1">
+        <f t="shared" ref="AN22:AP22" si="85">AM22/$E22</f>
         <v>0.60963930210388628</v>
       </c>
-      <c r="AK22">
+      <c r="AO22">
         <v>25852</v>
       </c>
-      <c r="AL22" s="1">
+      <c r="AP22" s="1">
         <f t="shared" si="85"/>
         <v>0.57312612233134552</v>
       </c>
-      <c r="AM22">
+      <c r="AQ22">
         <v>25553</v>
       </c>
-      <c r="AN22" s="1">
-        <f t="shared" ref="AN22:AP22" si="86">AM22/$E22</f>
+      <c r="AR22" s="1">
+        <f t="shared" ref="AR22:AT22" si="86">AQ22/$E22</f>
         <v>0.56649743942181918</v>
       </c>
-      <c r="AO22">
+      <c r="AS22">
         <v>26401</v>
       </c>
-      <c r="AP22" s="1">
+      <c r="AT22" s="1">
         <f t="shared" si="86"/>
         <v>0.58529718225552574</v>
       </c>
     </row>
-    <row r="23" spans="3:42" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>17</v>
       </c>
@@ -5872,67 +6466,86 @@
         <f t="shared" ref="W23" si="89">V23/$E23</f>
         <v>0.99758368432720013</v>
       </c>
-      <c r="X23" s="1"/>
-      <c r="Y23" s="1"/>
-      <c r="Z23" s="1"/>
-      <c r="AA23" s="10">
+      <c r="X23" s="24">
+        <v>45103</v>
+      </c>
+      <c r="Y23" s="25">
+        <f>X23/$E23</f>
+        <v>0.99984482376413208</v>
+      </c>
+      <c r="Z23" s="6">
+        <v>44904</v>
+      </c>
+      <c r="AA23" s="25">
+        <f>Z23/$E23</f>
+        <v>0.99543338505874523</v>
+      </c>
+      <c r="AB23">
+        <v>44920</v>
+      </c>
+      <c r="AC23" s="25">
+        <f>AB23/$E23</f>
+        <v>0.99578807359787191</v>
+      </c>
+      <c r="AD23" s="1"/>
+      <c r="AE23" s="10">
         <v>36911</v>
       </c>
-      <c r="AB23" s="11">
+      <c r="AF23" s="11">
         <f t="shared" si="6"/>
         <v>0.8182442917313234</v>
       </c>
-      <c r="AC23" s="12">
+      <c r="AG23" s="12">
         <v>36119</v>
       </c>
-      <c r="AD23" s="11">
+      <c r="AH23" s="11">
         <f t="shared" si="7"/>
         <v>0.8006872090445577</v>
       </c>
-      <c r="AE23" s="12">
+      <c r="AI23" s="12">
         <v>36439</v>
       </c>
-      <c r="AF23" s="11">
+      <c r="AJ23" s="11">
         <f t="shared" si="8"/>
         <v>0.8077809798270893</v>
       </c>
-      <c r="AG23" s="12">
+      <c r="AK23" s="12">
         <v>36505</v>
       </c>
-      <c r="AH23" s="13">
+      <c r="AL23" s="13">
         <f t="shared" si="9"/>
         <v>0.80924407005098653</v>
       </c>
-      <c r="AI23">
+      <c r="AM23">
         <v>26446</v>
       </c>
-      <c r="AJ23" s="1">
-        <f t="shared" ref="AJ23:AL23" si="90">AI23/$E23</f>
+      <c r="AN23" s="1">
+        <f t="shared" ref="AN23:AP23" si="90">AM23/$E23</f>
         <v>0.58625581910884506</v>
       </c>
-      <c r="AK23">
+      <c r="AO23">
         <v>26132</v>
       </c>
-      <c r="AL23" s="1">
+      <c r="AP23" s="1">
         <f t="shared" si="90"/>
         <v>0.5792950565284859</v>
       </c>
-      <c r="AM23">
+      <c r="AQ23">
         <v>26522</v>
       </c>
-      <c r="AN23" s="1">
-        <f t="shared" ref="AN23:AP23" si="91">AM23/$E23</f>
+      <c r="AR23" s="1">
+        <f t="shared" ref="AR23:AT23" si="91">AQ23/$E23</f>
         <v>0.58794058966969631</v>
       </c>
-      <c r="AO23">
+      <c r="AS23">
         <v>25574</v>
       </c>
-      <c r="AP23" s="1">
+      <c r="AT23" s="1">
         <f t="shared" si="91"/>
         <v>0.56692529372644651</v>
       </c>
     </row>
-    <row r="24" spans="3:42" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C24">
         <v>18</v>
       </c>
@@ -6005,67 +6618,86 @@
         <f t="shared" ref="W24" si="94">V24/$E24</f>
         <v>0.99760590543326466</v>
       </c>
-      <c r="X24" s="1"/>
-      <c r="Y24" s="1"/>
-      <c r="Z24" s="1"/>
-      <c r="AA24" s="10">
+      <c r="X24" s="24">
+        <v>45098</v>
+      </c>
+      <c r="Y24" s="25">
+        <f>X24/$E24</f>
+        <v>0.99971182195030039</v>
+      </c>
+      <c r="Z24" s="6">
+        <v>44904</v>
+      </c>
+      <c r="AA24" s="25">
+        <f>Z24/$E24</f>
+        <v>0.99541131874709055</v>
+      </c>
+      <c r="AB24">
+        <v>44920</v>
+      </c>
+      <c r="AC24" s="25">
+        <f>AB24/$E24</f>
+        <v>0.99576599942364385</v>
+      </c>
+      <c r="AD24" s="1"/>
+      <c r="AE24" s="10">
         <v>37032</v>
       </c>
-      <c r="AB24" s="11">
+      <c r="AF24" s="11">
         <f t="shared" si="6"/>
         <v>0.82090842588282242</v>
       </c>
-      <c r="AC24" s="12">
+      <c r="AG24" s="12">
         <v>35878</v>
       </c>
-      <c r="AD24" s="11">
+      <c r="AH24" s="11">
         <f t="shared" si="7"/>
         <v>0.79532708208640912</v>
       </c>
-      <c r="AE24" s="12">
+      <c r="AI24" s="12">
         <v>36347</v>
       </c>
-      <c r="AF24" s="11">
+      <c r="AJ24" s="11">
         <f t="shared" si="8"/>
         <v>0.80572365941788038</v>
       </c>
-      <c r="AG24" s="12">
+      <c r="AK24" s="12">
         <v>36513</v>
       </c>
-      <c r="AH24" s="13">
+      <c r="AL24" s="13">
         <f t="shared" si="9"/>
         <v>0.80940347143712177</v>
       </c>
-      <c r="AI24">
+      <c r="AM24">
         <v>25149</v>
       </c>
-      <c r="AJ24" s="1">
-        <f t="shared" ref="AJ24:AL24" si="95">AI24/$E24</f>
+      <c r="AN24" s="1">
+        <f t="shared" ref="AN24:AP24" si="95">AM24/$E24</f>
         <v>0.55749152091507614</v>
       </c>
-      <c r="AK24">
+      <c r="AO24">
         <v>26325</v>
       </c>
-      <c r="AL24" s="1">
+      <c r="AP24" s="1">
         <f t="shared" si="95"/>
         <v>0.58356055064175039</v>
       </c>
-      <c r="AM24">
+      <c r="AQ24">
         <v>26476</v>
       </c>
-      <c r="AN24" s="1">
-        <f t="shared" ref="AN24:AP24" si="96">AM24/$E24</f>
+      <c r="AR24" s="1">
+        <f t="shared" ref="AR24:AT24" si="96">AQ24/$E24</f>
         <v>0.58690784952672292</v>
       </c>
-      <c r="AO24">
+      <c r="AS24">
         <v>26063</v>
       </c>
-      <c r="AP24" s="1">
+      <c r="AT24" s="1">
         <f t="shared" si="96"/>
         <v>0.57775265456318858</v>
       </c>
     </row>
-    <row r="25" spans="3:42" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C25">
         <v>19</v>
       </c>
@@ -6138,67 +6770,86 @@
         <f t="shared" ref="W25" si="99">V25/$E25</f>
         <v>0.99762796781130147</v>
       </c>
-      <c r="X25" s="1"/>
-      <c r="Y25" s="1"/>
-      <c r="Z25" s="1"/>
-      <c r="AA25" s="10">
+      <c r="X25" s="24">
+        <v>45091</v>
+      </c>
+      <c r="Y25" s="25">
+        <f>X25/$E25</f>
+        <v>0.99960096654769559</v>
+      </c>
+      <c r="Z25" s="6">
+        <v>44904</v>
+      </c>
+      <c r="AA25" s="25">
+        <f>Z25/$E25</f>
+        <v>0.99545545234875521</v>
+      </c>
+      <c r="AB25">
+        <v>44920</v>
+      </c>
+      <c r="AC25" s="25">
+        <f>AB25/$E25</f>
+        <v>0.99581014875080365</v>
+      </c>
+      <c r="AD25" s="1"/>
+      <c r="AE25" s="10">
         <v>37569</v>
       </c>
-      <c r="AB25" s="11">
+      <c r="AF25" s="11">
         <f t="shared" si="6"/>
         <v>0.83284932053470484</v>
       </c>
-      <c r="AC25" s="12">
+      <c r="AG25" s="12">
         <v>36807</v>
       </c>
-      <c r="AD25" s="11">
+      <c r="AH25" s="11">
         <f t="shared" si="7"/>
         <v>0.81595690438715107</v>
       </c>
-      <c r="AE25" s="12">
+      <c r="AI25" s="12">
         <v>36789</v>
       </c>
-      <c r="AF25" s="11">
+      <c r="AJ25" s="11">
         <f t="shared" si="8"/>
         <v>0.81555787093484666</v>
       </c>
-      <c r="AG25" s="12">
+      <c r="AK25" s="12">
         <v>36577</v>
       </c>
-      <c r="AH25" s="13">
+      <c r="AL25" s="13">
         <f t="shared" si="9"/>
         <v>0.81085814360770581</v>
       </c>
-      <c r="AI25">
+      <c r="AM25">
         <v>25817</v>
       </c>
-      <c r="AJ25" s="1">
-        <f t="shared" ref="AJ25:AL25" si="100">AI25/$E25</f>
+      <c r="AN25" s="1">
+        <f t="shared" ref="AN25:AP25" si="100">AM25/$E25</f>
         <v>0.57232481323017581</v>
       </c>
-      <c r="AK25">
+      <c r="AO25">
         <v>25803</v>
       </c>
-      <c r="AL25" s="1">
+      <c r="AP25" s="1">
         <f t="shared" si="100"/>
         <v>0.57201445387838346</v>
       </c>
-      <c r="AM25">
+      <c r="AQ25">
         <v>25729</v>
       </c>
-      <c r="AN25" s="1">
-        <f t="shared" ref="AN25:AP25" si="101">AM25/$E25</f>
+      <c r="AR25" s="1">
+        <f t="shared" ref="AR25:AT25" si="101">AQ25/$E25</f>
         <v>0.57037398301890974</v>
       </c>
-      <c r="AO25">
+      <c r="AS25">
         <v>26210</v>
       </c>
-      <c r="AP25" s="1">
+      <c r="AT25" s="1">
         <f t="shared" si="101"/>
         <v>0.58103704360548891</v>
       </c>
     </row>
-    <row r="26" spans="3:42" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>20</v>
       </c>
@@ -6271,67 +6922,86 @@
         <f t="shared" ref="W26" si="104">V26/$E26</f>
         <v>0.99592117221963605</v>
       </c>
-      <c r="X26" s="1"/>
-      <c r="Y26" s="1"/>
-      <c r="Z26" s="1"/>
-      <c r="AA26" s="10">
+      <c r="X26" s="24">
+        <v>43466</v>
+      </c>
+      <c r="Y26" s="25">
+        <f>X26/$E26</f>
+        <v>0.9635343929418545</v>
+      </c>
+      <c r="Z26" s="6">
+        <v>44903</v>
+      </c>
+      <c r="AA26" s="25">
+        <f>Z26/$E26</f>
+        <v>0.99538915120480598</v>
+      </c>
+      <c r="AB26">
+        <v>44919</v>
+      </c>
+      <c r="AC26" s="25">
+        <f>AB26/$E26</f>
+        <v>0.99574383188135929</v>
+      </c>
+      <c r="AD26" s="1"/>
+      <c r="AE26" s="10">
         <v>36647</v>
       </c>
-      <c r="AB26" s="11">
+      <c r="AF26" s="11">
         <f t="shared" si="6"/>
         <v>0.81237392210325643</v>
       </c>
-      <c r="AC26" s="12">
+      <c r="AG26" s="12">
         <v>33236</v>
       </c>
-      <c r="AD26" s="11">
+      <c r="AH26" s="11">
         <f t="shared" si="7"/>
         <v>0.73676043537053049</v>
       </c>
-      <c r="AE26" s="12">
+      <c r="AI26" s="12">
         <v>35105</v>
       </c>
-      <c r="AF26" s="11">
+      <c r="AJ26" s="11">
         <f t="shared" si="8"/>
         <v>0.77819157190042343</v>
       </c>
-      <c r="AG26" s="12">
+      <c r="AK26" s="12">
         <v>33872</v>
       </c>
-      <c r="AH26" s="13">
+      <c r="AL26" s="13">
         <f t="shared" si="9"/>
         <v>0.7508589922635277</v>
       </c>
-      <c r="AI26">
+      <c r="AM26">
         <v>39785</v>
       </c>
-      <c r="AJ26" s="1">
-        <f t="shared" ref="AJ26:AL26" si="105">AI26/$E26</f>
+      <c r="AN26" s="1">
+        <f t="shared" ref="AN26:AP26" si="105">AM26/$E26</f>
         <v>0.8819356697922901</v>
       </c>
-      <c r="AK26">
+      <c r="AO26">
         <v>40037</v>
       </c>
-      <c r="AL26" s="1">
+      <c r="AP26" s="1">
         <f t="shared" si="105"/>
         <v>0.887521890448006</v>
       </c>
-      <c r="AM26">
+      <c r="AQ26">
         <v>40368</v>
       </c>
-      <c r="AN26" s="1">
-        <f t="shared" ref="AN26:AP26" si="106">AM26/$E26</f>
+      <c r="AR26" s="1">
+        <f t="shared" ref="AR26:AT26" si="106">AQ26/$E26</f>
         <v>0.89485934694420433</v>
       </c>
-      <c r="AO26">
+      <c r="AS26">
         <v>40071</v>
       </c>
-      <c r="AP26" s="1">
+      <c r="AT26" s="1">
         <f t="shared" si="106"/>
         <v>0.88827558688568198</v>
       </c>
     </row>
-    <row r="27" spans="3:42" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C27">
         <v>21</v>
       </c>
@@ -6404,67 +7074,86 @@
         <f t="shared" ref="W27" si="109">V27/$E27</f>
         <v>0.99769437116190396</v>
       </c>
-      <c r="X27" s="1"/>
-      <c r="Y27" s="1"/>
-      <c r="Z27" s="1"/>
-      <c r="AA27" s="10">
+      <c r="X27" s="24">
+        <v>45105</v>
+      </c>
+      <c r="Y27" s="25">
+        <f>X27/$E27</f>
+        <v>0.99995566098388278</v>
+      </c>
+      <c r="Z27" s="6">
+        <v>44904</v>
+      </c>
+      <c r="AA27" s="25">
+        <f>Z27/$E27</f>
+        <v>0.99549958986410092</v>
+      </c>
+      <c r="AB27">
+        <v>44920</v>
+      </c>
+      <c r="AC27" s="25">
+        <f>AB27/$E27</f>
+        <v>0.99585430199303882</v>
+      </c>
+      <c r="AD27" s="1"/>
+      <c r="AE27" s="10">
         <v>39684</v>
       </c>
-      <c r="AB27" s="11">
+      <c r="AF27" s="11">
         <f t="shared" si="6"/>
         <v>0.87977475779812442</v>
       </c>
-      <c r="AC27" s="12">
+      <c r="AG27" s="12">
         <v>38817</v>
       </c>
-      <c r="AD27" s="11">
+      <c r="AH27" s="11">
         <f t="shared" si="7"/>
         <v>0.86055379431130419</v>
       </c>
-      <c r="AE27" s="12">
+      <c r="AI27" s="12">
         <v>38854</v>
       </c>
-      <c r="AF27" s="11">
+      <c r="AJ27" s="11">
         <f t="shared" si="8"/>
         <v>0.86137406610947298</v>
       </c>
-      <c r="AG27" s="12">
+      <c r="AK27" s="12">
         <v>38597</v>
       </c>
-      <c r="AH27" s="13">
+      <c r="AL27" s="13">
         <f t="shared" si="9"/>
         <v>0.85567650253840866</v>
       </c>
-      <c r="AI27">
+      <c r="AM27">
         <v>27630</v>
       </c>
-      <c r="AJ27" s="1">
-        <f t="shared" ref="AJ27:AL27" si="110">AI27/$E27</f>
+      <c r="AN27" s="1">
+        <f t="shared" ref="AN27:AP27" si="110">AM27/$E27</f>
         <v>0.612543507659565</v>
       </c>
-      <c r="AK27">
+      <c r="AO27">
         <v>26048</v>
       </c>
-      <c r="AL27" s="1">
+      <c r="AP27" s="1">
         <f t="shared" si="110"/>
         <v>0.57747134591083427</v>
       </c>
-      <c r="AM27">
+      <c r="AQ27">
         <v>25483</v>
       </c>
-      <c r="AN27" s="1">
-        <f t="shared" ref="AN27:AP27" si="111">AM27/$E27</f>
+      <c r="AR27" s="1">
+        <f t="shared" ref="AR27:AT27" si="111">AQ27/$E27</f>
         <v>0.56494557385771604</v>
       </c>
-      <c r="AO27">
+      <c r="AS27">
         <v>26249</v>
       </c>
-      <c r="AP27" s="1">
+      <c r="AT27" s="1">
         <f t="shared" si="111"/>
         <v>0.58192741703061612</v>
       </c>
     </row>
-    <row r="28" spans="3:42" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C28">
         <v>22</v>
       </c>
@@ -6537,67 +7226,86 @@
         <f t="shared" ref="W28" si="114">V28/$E28</f>
         <v>0.99758368432720013</v>
       </c>
-      <c r="X28" s="1"/>
-      <c r="Y28" s="1"/>
-      <c r="Z28" s="1"/>
-      <c r="AA28" s="10">
+      <c r="X28" s="24">
+        <v>45102</v>
+      </c>
+      <c r="Y28" s="25">
+        <f>X28/$E28</f>
+        <v>0.99982265573043672</v>
+      </c>
+      <c r="Z28" s="6">
+        <v>44904</v>
+      </c>
+      <c r="AA28" s="25">
+        <f>Z28/$E28</f>
+        <v>0.99543338505874523</v>
+      </c>
+      <c r="AB28">
+        <v>44920</v>
+      </c>
+      <c r="AC28" s="25">
+        <f>AB28/$E28</f>
+        <v>0.99578807359787191</v>
+      </c>
+      <c r="AD28" s="1"/>
+      <c r="AE28" s="10">
         <v>41572</v>
       </c>
-      <c r="AB28" s="11">
+      <c r="AF28" s="11">
         <f t="shared" si="6"/>
         <v>0.92156949678563516</v>
       </c>
-      <c r="AC28" s="12">
+      <c r="AG28" s="12">
         <v>40819</v>
       </c>
-      <c r="AD28" s="11">
+      <c r="AH28" s="11">
         <f t="shared" si="7"/>
         <v>0.90487696741299051</v>
       </c>
-      <c r="AE28" s="12">
+      <c r="AI28" s="12">
         <v>40338</v>
       </c>
-      <c r="AF28" s="11">
+      <c r="AJ28" s="11">
         <f t="shared" si="8"/>
         <v>0.89421414320549764</v>
       </c>
-      <c r="AG28" s="12">
+      <c r="AK28" s="12">
         <v>40323</v>
       </c>
-      <c r="AH28" s="13">
+      <c r="AL28" s="13">
         <f t="shared" si="9"/>
         <v>0.89388162270006655</v>
       </c>
-      <c r="AI28">
+      <c r="AM28">
         <v>26578</v>
       </c>
-      <c r="AJ28" s="1">
-        <f t="shared" ref="AJ28:AL28" si="115">AI28/$E28</f>
+      <c r="AN28" s="1">
+        <f t="shared" ref="AN28:AP28" si="115">AM28/$E28</f>
         <v>0.5891819995566393</v>
       </c>
-      <c r="AK28">
+      <c r="AO28">
         <v>26520</v>
       </c>
-      <c r="AL28" s="1">
+      <c r="AP28" s="1">
         <f t="shared" si="115"/>
         <v>0.58789625360230546</v>
       </c>
-      <c r="AM28">
+      <c r="AQ28">
         <v>27223</v>
       </c>
-      <c r="AN28" s="1">
-        <f t="shared" ref="AN28:AP28" si="116">AM28/$E28</f>
+      <c r="AR28" s="1">
+        <f t="shared" ref="AR28:AT28" si="116">AQ28/$E28</f>
         <v>0.60348038129017956</v>
       </c>
-      <c r="AO28">
+      <c r="AS28">
         <v>26227</v>
       </c>
-      <c r="AP28" s="1">
+      <c r="AT28" s="1">
         <f t="shared" si="116"/>
         <v>0.58140101972954994</v>
       </c>
     </row>
-    <row r="29" spans="3:42" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C29">
         <v>23</v>
       </c>
@@ -6670,67 +7378,86 @@
         <f t="shared" ref="W29" si="119">V29/$E29</f>
         <v>0.99760590543326466</v>
       </c>
-      <c r="X29" s="1"/>
-      <c r="Y29" s="1"/>
-      <c r="Z29" s="1"/>
-      <c r="AA29" s="10">
+      <c r="X29" s="24">
+        <v>45109</v>
+      </c>
+      <c r="Y29" s="25">
+        <f>X29/$E29</f>
+        <v>0.99995566491543086</v>
+      </c>
+      <c r="Z29" s="6">
+        <v>44904</v>
+      </c>
+      <c r="AA29" s="25">
+        <f>Z29/$E29</f>
+        <v>0.99541131874709055</v>
+      </c>
+      <c r="AB29">
+        <v>44920</v>
+      </c>
+      <c r="AC29" s="25">
+        <f>AB29/$E29</f>
+        <v>0.99576599942364385</v>
+      </c>
+      <c r="AD29" s="1"/>
+      <c r="AE29" s="10">
         <v>41846</v>
       </c>
-      <c r="AB29" s="11">
+      <c r="AF29" s="11">
         <f t="shared" si="6"/>
         <v>0.92762297444082376</v>
       </c>
-      <c r="AC29" s="12">
+      <c r="AG29" s="12">
         <v>40896</v>
       </c>
-      <c r="AD29" s="11">
+      <c r="AH29" s="11">
         <f t="shared" si="7"/>
         <v>0.9065638092704662</v>
       </c>
-      <c r="AE29" s="12">
+      <c r="AI29" s="12">
         <v>40756</v>
       </c>
-      <c r="AF29" s="11">
+      <c r="AJ29" s="11">
         <f t="shared" si="8"/>
         <v>0.90346035335062402</v>
       </c>
-      <c r="AG29" s="12">
+      <c r="AK29" s="12">
         <v>40688</v>
       </c>
-      <c r="AH29" s="13">
+      <c r="AL29" s="13">
         <f t="shared" si="9"/>
         <v>0.90195296047527207</v>
       </c>
-      <c r="AI29">
+      <c r="AM29">
         <v>25630</v>
       </c>
-      <c r="AJ29" s="1">
-        <f t="shared" ref="AJ29:AL29" si="120">AI29/$E29</f>
+      <c r="AN29" s="1">
+        <f t="shared" ref="AN29:AP29" si="120">AM29/$E29</f>
         <v>0.56815410875396244</v>
       </c>
-      <c r="AK29">
+      <c r="AO29">
         <v>26788</v>
       </c>
-      <c r="AL29" s="1">
+      <c r="AP29" s="1">
         <f t="shared" si="120"/>
         <v>0.59382412271951412</v>
       </c>
-      <c r="AM29">
+      <c r="AQ29">
         <v>26781</v>
       </c>
-      <c r="AN29" s="1">
-        <f t="shared" ref="AN29:AP29" si="121">AM29/$E29</f>
+      <c r="AR29" s="1">
+        <f t="shared" ref="AR29:AT29" si="121">AQ29/$E29</f>
         <v>0.59366894992352193</v>
       </c>
-      <c r="AO29">
+      <c r="AS29">
         <v>26476</v>
       </c>
-      <c r="AP29" s="1">
+      <c r="AT29" s="1">
         <f t="shared" si="121"/>
         <v>0.58690784952672292</v>
       </c>
     </row>
-    <row r="30" spans="3:42" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C30">
         <v>24</v>
       </c>
@@ -6803,67 +7530,86 @@
         <f t="shared" ref="W30" si="124">V30/$E30</f>
         <v>0.99765013633642952</v>
       </c>
-      <c r="X30" s="1"/>
-      <c r="Y30" s="1"/>
-      <c r="Z30" s="1"/>
-      <c r="AA30" s="10">
+      <c r="X30" s="24">
+        <v>45108</v>
+      </c>
+      <c r="Y30" s="25">
+        <f>X30/$E30</f>
+        <v>0.99997783147487196</v>
+      </c>
+      <c r="Z30" s="6">
+        <v>44904</v>
+      </c>
+      <c r="AA30" s="25">
+        <f>Z30/$E30</f>
+        <v>0.99545545234875521</v>
+      </c>
+      <c r="AB30">
+        <v>44920</v>
+      </c>
+      <c r="AC30" s="25">
+        <f>AB30/$E30</f>
+        <v>0.99581014875080365</v>
+      </c>
+      <c r="AD30" s="1"/>
+      <c r="AE30" s="10">
         <v>41464</v>
       </c>
-      <c r="AB30" s="11">
+      <c r="AF30" s="11">
         <f t="shared" si="6"/>
         <v>0.9191957259083553</v>
       </c>
-      <c r="AC30" s="12">
+      <c r="AG30" s="12">
         <v>40242</v>
       </c>
-      <c r="AD30" s="11">
+      <c r="AH30" s="11">
         <f t="shared" si="7"/>
         <v>0.89210578820191089</v>
       </c>
-      <c r="AE30" s="12">
+      <c r="AI30" s="12">
         <v>40275</v>
       </c>
-      <c r="AF30" s="11">
+      <c r="AJ30" s="11">
         <f t="shared" si="8"/>
         <v>0.89283734953113569</v>
       </c>
-      <c r="AG30" s="12">
+      <c r="AK30" s="12">
         <v>39998</v>
       </c>
-      <c r="AH30" s="13">
+      <c r="AL30" s="13">
         <f t="shared" si="9"/>
         <v>0.88669666807067327</v>
       </c>
-      <c r="AI30">
+      <c r="AM30">
         <v>26888</v>
       </c>
-      <c r="AJ30" s="1">
-        <f t="shared" ref="AJ30:AL30" si="125">AI30/$E30</f>
+      <c r="AN30" s="1">
+        <f t="shared" ref="AN30:AP30" si="125">AM30/$E30</f>
         <v>0.59606730364228866</v>
       </c>
-      <c r="AK30">
+      <c r="AO30">
         <v>26317</v>
       </c>
-      <c r="AL30" s="1">
+      <c r="AP30" s="1">
         <f t="shared" si="125"/>
         <v>0.58340907579418744</v>
       </c>
-      <c r="AM30">
+      <c r="AQ30">
         <v>26009</v>
       </c>
-      <c r="AN30" s="1">
-        <f t="shared" ref="AN30:AP30" si="126">AM30/$E30</f>
+      <c r="AR30" s="1">
+        <f t="shared" ref="AR30:AT30" si="126">AQ30/$E30</f>
         <v>0.57658117005475629</v>
       </c>
-      <c r="AO30">
+      <c r="AS30">
         <v>26685</v>
       </c>
-      <c r="AP30" s="1">
+      <c r="AT30" s="1">
         <f t="shared" si="126"/>
         <v>0.59156709304129995</v>
       </c>
     </row>
-    <row r="31" spans="3:42" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C31">
         <v>25</v>
       </c>
@@ -6936,67 +7682,86 @@
         <f t="shared" ref="W31" si="129">V31/$E31</f>
         <v>0.99765003214578674</v>
       </c>
-      <c r="X31" s="1"/>
-      <c r="Y31" s="1"/>
-      <c r="Z31" s="1"/>
-      <c r="AA31" s="10">
+      <c r="X31" s="24">
+        <v>45101</v>
+      </c>
+      <c r="Y31" s="25">
+        <f>X31/$E31</f>
+        <v>0.99986698295164833</v>
+      </c>
+      <c r="Z31" s="6">
+        <v>44904</v>
+      </c>
+      <c r="AA31" s="25">
+        <f>Z31/$E31</f>
+        <v>0.99549958986410092</v>
+      </c>
+      <c r="AB31">
+        <v>44920</v>
+      </c>
+      <c r="AC31" s="25">
+        <f>AB31/$E31</f>
+        <v>0.99585430199303882</v>
+      </c>
+      <c r="AD31" s="1"/>
+      <c r="AE31" s="10">
         <v>39284</v>
       </c>
-      <c r="AB31" s="11">
+      <c r="AF31" s="11">
         <f t="shared" si="6"/>
         <v>0.87090695457467804</v>
       </c>
-      <c r="AC31" s="12">
+      <c r="AG31" s="12">
         <v>38286</v>
       </c>
-      <c r="AD31" s="11">
+      <c r="AH31" s="11">
         <f t="shared" si="7"/>
         <v>0.84878178553217909</v>
       </c>
-      <c r="AE31" s="12">
+      <c r="AI31" s="12">
         <v>38127</v>
       </c>
-      <c r="AF31" s="11">
+      <c r="AJ31" s="11">
         <f t="shared" si="8"/>
         <v>0.84525683375085903</v>
       </c>
-      <c r="AG31" s="12">
+      <c r="AK31" s="12">
         <v>37984</v>
       </c>
-      <c r="AH31" s="13">
+      <c r="AL31" s="13">
         <f t="shared" si="9"/>
         <v>0.84208659409847697</v>
       </c>
-      <c r="AI31">
+      <c r="AM31">
         <v>27196</v>
       </c>
-      <c r="AJ31" s="1">
-        <f t="shared" ref="AJ31:AL31" si="130">AI31/$E31</f>
+      <c r="AN31" s="1">
+        <f t="shared" ref="AN31:AP31" si="130">AM31/$E31</f>
         <v>0.60292194116212561</v>
       </c>
-      <c r="AK31">
+      <c r="AO31">
         <v>25969</v>
       </c>
-      <c r="AL31" s="1">
+      <c r="AP31" s="1">
         <f t="shared" si="130"/>
         <v>0.57571995477420357</v>
       </c>
-      <c r="AM31">
+      <c r="AQ31">
         <v>25430</v>
       </c>
-      <c r="AN31" s="1">
-        <f t="shared" ref="AN31:AP31" si="131">AM31/$E31</f>
+      <c r="AR31" s="1">
+        <f t="shared" ref="AR31:AT31" si="131">AQ31/$E31</f>
         <v>0.56377058993060947</v>
       </c>
-      <c r="AO31">
+      <c r="AS31">
         <v>25911</v>
       </c>
-      <c r="AP31" s="1">
+      <c r="AT31" s="1">
         <f t="shared" si="131"/>
         <v>0.57443412330680377</v>
       </c>
     </row>
-    <row r="32" spans="3:42" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C32">
         <v>26</v>
       </c>
@@ -7069,67 +7834,86 @@
         <f t="shared" ref="W32" si="134">V32/$E32</f>
         <v>0.99762802039459098</v>
       </c>
-      <c r="X32" s="1"/>
-      <c r="Y32" s="1"/>
-      <c r="Z32" s="1"/>
-      <c r="AA32" s="10">
+      <c r="X32" s="24">
+        <v>45101</v>
+      </c>
+      <c r="Y32" s="25">
+        <f>X32/$E32</f>
+        <v>0.99980048769674135</v>
+      </c>
+      <c r="Z32" s="6">
+        <v>44904</v>
+      </c>
+      <c r="AA32" s="25">
+        <f>Z32/$E32</f>
+        <v>0.99543338505874523</v>
+      </c>
+      <c r="AB32">
+        <v>44920</v>
+      </c>
+      <c r="AC32" s="25">
+        <f>AB32/$E32</f>
+        <v>0.99578807359787191</v>
+      </c>
+      <c r="AD32" s="1"/>
+      <c r="AE32" s="10">
         <v>38438</v>
       </c>
-      <c r="AB32" s="11">
+      <c r="AF32" s="11">
         <f t="shared" si="6"/>
         <v>0.85209487918421634</v>
       </c>
-      <c r="AC32" s="12">
+      <c r="AG32" s="12">
         <v>37638</v>
       </c>
-      <c r="AD32" s="11">
+      <c r="AH32" s="11">
         <f t="shared" si="7"/>
         <v>0.83436045222788735</v>
       </c>
-      <c r="AE32" s="12">
+      <c r="AI32" s="12">
         <v>37394</v>
       </c>
-      <c r="AF32" s="11">
+      <c r="AJ32" s="11">
         <f t="shared" si="8"/>
         <v>0.82895145200620701</v>
       </c>
-      <c r="AG32" s="12">
+      <c r="AK32" s="12">
         <v>37617</v>
       </c>
-      <c r="AH32" s="13">
+      <c r="AL32" s="13">
         <f t="shared" si="9"/>
         <v>0.83389492352028372</v>
       </c>
-      <c r="AI32">
+      <c r="AM32">
         <v>25505</v>
       </c>
-      <c r="AJ32" s="1">
-        <f t="shared" ref="AJ32:AL32" si="135">AI32/$E32</f>
+      <c r="AN32" s="1">
+        <f t="shared" ref="AN32:AP32" si="135">AM32/$E32</f>
         <v>0.56539569940146306</v>
       </c>
-      <c r="AK32">
+      <c r="AO32">
         <v>25891</v>
       </c>
-      <c r="AL32" s="1">
+      <c r="AP32" s="1">
         <f t="shared" si="135"/>
         <v>0.57395256040789178</v>
       </c>
-      <c r="AM32">
+      <c r="AQ32">
         <v>26703</v>
       </c>
-      <c r="AN32" s="1">
-        <f t="shared" ref="AN32:AP32" si="136">AM32/$E32</f>
+      <c r="AR32" s="1">
+        <f t="shared" ref="AR32:AT32" si="136">AQ32/$E32</f>
         <v>0.59195300376856574</v>
       </c>
-      <c r="AO32">
+      <c r="AS32">
         <v>25701</v>
       </c>
-      <c r="AP32" s="1">
+      <c r="AT32" s="1">
         <f t="shared" si="136"/>
         <v>0.56974063400576369</v>
       </c>
     </row>
-    <row r="33" spans="3:42" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C33">
         <v>27</v>
       </c>
@@ -7202,67 +7986,86 @@
         <f t="shared" ref="W33" si="139">V33/$E33</f>
         <v>0.99760590543326466</v>
       </c>
-      <c r="X33" s="1"/>
-      <c r="Y33" s="1"/>
-      <c r="Z33" s="1"/>
-      <c r="AA33" s="10">
+      <c r="X33" s="24">
+        <v>45109</v>
+      </c>
+      <c r="Y33" s="25">
+        <f>X33/$E33</f>
+        <v>0.99995566491543086</v>
+      </c>
+      <c r="Z33" s="6">
+        <v>44904</v>
+      </c>
+      <c r="AA33" s="25">
+        <f>Z33/$E33</f>
+        <v>0.99541131874709055</v>
+      </c>
+      <c r="AB33">
+        <v>44920</v>
+      </c>
+      <c r="AC33" s="25">
+        <f>AB33/$E33</f>
+        <v>0.99576599942364385</v>
+      </c>
+      <c r="AD33" s="1"/>
+      <c r="AE33" s="10">
         <v>39377</v>
       </c>
-      <c r="AB33" s="11">
+      <c r="AF33" s="11">
         <f t="shared" si="6"/>
         <v>0.87289131254017871</v>
       </c>
-      <c r="AC33" s="12">
+      <c r="AG33" s="12">
         <v>37911</v>
       </c>
-      <c r="AD33" s="11">
+      <c r="AH33" s="11">
         <f t="shared" si="7"/>
         <v>0.84039369555097432</v>
       </c>
-      <c r="AE33" s="12">
+      <c r="AI33" s="12">
         <v>38306</v>
       </c>
-      <c r="AF33" s="11">
+      <c r="AJ33" s="11">
         <f t="shared" si="8"/>
         <v>0.8491498747533861</v>
       </c>
-      <c r="AG33" s="12">
+      <c r="AK33" s="12">
         <v>38214</v>
       </c>
-      <c r="AH33" s="13">
+      <c r="AL33" s="13">
         <f t="shared" si="9"/>
         <v>0.84711046086320407</v>
       </c>
-      <c r="AI33">
+      <c r="AM33">
         <v>24723</v>
       </c>
-      <c r="AJ33" s="1">
-        <f t="shared" ref="AJ33:AL33" si="140">AI33/$E33</f>
+      <c r="AN33" s="1">
+        <f t="shared" ref="AN33:AP33" si="140">AM33/$E33</f>
         <v>0.54804814790184209</v>
       </c>
-      <c r="AK33">
+      <c r="AO33">
         <v>26088</v>
       </c>
-      <c r="AL33" s="1">
+      <c r="AP33" s="1">
         <f t="shared" si="140"/>
         <v>0.57830684312030323</v>
       </c>
-      <c r="AM33">
+      <c r="AQ33">
         <v>26031</v>
       </c>
-      <c r="AN33" s="1">
-        <f t="shared" ref="AN33:AP33" si="141">AM33/$E33</f>
+      <c r="AR33" s="1">
+        <f t="shared" ref="AR33:AT33" si="141">AQ33/$E33</f>
         <v>0.57704329321008185</v>
       </c>
-      <c r="AO33">
+      <c r="AS33">
         <v>25791</v>
       </c>
-      <c r="AP33" s="1">
+      <c r="AT33" s="1">
         <f t="shared" si="141"/>
         <v>0.57172308306178099</v>
       </c>
     </row>
-    <row r="34" spans="3:42" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C34">
         <v>28</v>
       </c>
@@ -7335,67 +8138,86 @@
         <f t="shared" ref="W34" si="144">V34/$E34</f>
         <v>0.99762796781130147</v>
       </c>
-      <c r="X34" s="1"/>
-      <c r="Y34" s="1"/>
-      <c r="Z34" s="1"/>
-      <c r="AA34" s="10">
+      <c r="X34" s="24">
+        <v>45107</v>
+      </c>
+      <c r="Y34" s="25">
+        <f>X34/$E34</f>
+        <v>0.99995566294974392</v>
+      </c>
+      <c r="Z34" s="6">
+        <v>44904</v>
+      </c>
+      <c r="AA34" s="25">
+        <f>Z34/$E34</f>
+        <v>0.99545545234875521</v>
+      </c>
+      <c r="AB34">
+        <v>44920</v>
+      </c>
+      <c r="AC34" s="25">
+        <f>AB34/$E34</f>
+        <v>0.99581014875080365</v>
+      </c>
+      <c r="AD34" s="1"/>
+      <c r="AE34" s="10">
         <v>39898</v>
       </c>
-      <c r="AB34" s="11">
+      <c r="AF34" s="11">
         <f t="shared" si="6"/>
         <v>0.88447981555787092</v>
       </c>
-      <c r="AC34" s="12">
+      <c r="AG34" s="12">
         <v>39259</v>
       </c>
-      <c r="AD34" s="11">
+      <c r="AH34" s="11">
         <f t="shared" si="7"/>
         <v>0.87031412800106411</v>
       </c>
-      <c r="AE34" s="12">
+      <c r="AI34" s="12">
         <v>39021</v>
       </c>
-      <c r="AF34" s="11">
+      <c r="AJ34" s="11">
         <f t="shared" si="8"/>
         <v>0.86503801902059452</v>
       </c>
-      <c r="AG34" s="12">
+      <c r="AK34" s="12">
         <v>39077</v>
       </c>
-      <c r="AH34" s="13">
+      <c r="AL34" s="13">
         <f t="shared" si="9"/>
         <v>0.86627945642776383</v>
       </c>
-      <c r="AI34">
+      <c r="AM34">
         <v>26404</v>
       </c>
-      <c r="AJ34" s="1">
-        <f t="shared" ref="AJ34:AL34" si="145">AI34/$E34</f>
+      <c r="AN34" s="1">
+        <f t="shared" ref="AN34:AP34" si="145">AM34/$E34</f>
         <v>0.58533773748032547</v>
       </c>
-      <c r="AK34">
+      <c r="AO34">
         <v>25413</v>
       </c>
-      <c r="AL34" s="1">
+      <c r="AP34" s="1">
         <f t="shared" si="145"/>
         <v>0.56336872907845437</v>
       </c>
-      <c r="AM34">
+      <c r="AQ34">
         <v>25077</v>
       </c>
-      <c r="AN34" s="1">
-        <f t="shared" ref="AN34:AP34" si="146">AM34/$E34</f>
+      <c r="AR34" s="1">
+        <f t="shared" ref="AR34:AT34" si="146">AQ34/$E34</f>
         <v>0.55592010463543862</v>
       </c>
-      <c r="AO34">
+      <c r="AS34">
         <v>25956</v>
       </c>
-      <c r="AP34" s="1">
+      <c r="AT34" s="1">
         <f t="shared" si="146"/>
         <v>0.57540623822297099</v>
       </c>
     </row>
-    <row r="35" spans="3:42" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C35">
         <v>29</v>
       </c>
@@ -7468,67 +8290,86 @@
         <f t="shared" ref="W35" si="149">V35/$E35</f>
         <v>0.99423375471279662</v>
       </c>
-      <c r="X35" s="1"/>
-      <c r="Y35" s="1"/>
-      <c r="Z35" s="1"/>
-      <c r="AA35" s="10">
+      <c r="X35" s="24">
+        <v>8951</v>
+      </c>
+      <c r="Y35" s="25">
+        <f>X35/$E35</f>
+        <v>0.9925704147261033</v>
+      </c>
+      <c r="Z35" s="6">
+        <v>8932</v>
+      </c>
+      <c r="AA35" s="25">
+        <f>Z35/$E35</f>
+        <v>0.99046351740962524</v>
+      </c>
+      <c r="AB35">
+        <v>8942</v>
+      </c>
+      <c r="AC35" s="25">
+        <f>AB35/$E35</f>
+        <v>0.99157241073408742</v>
+      </c>
+      <c r="AD35" s="1"/>
+      <c r="AE35" s="10">
         <v>8051</v>
       </c>
-      <c r="AB35" s="11">
+      <c r="AF35" s="11">
         <f t="shared" si="6"/>
         <v>0.89277001552450652</v>
       </c>
-      <c r="AC35" s="12">
+      <c r="AG35" s="12">
         <v>7883</v>
       </c>
-      <c r="AD35" s="11">
+      <c r="AH35" s="11">
         <f t="shared" si="7"/>
         <v>0.87414060767354185</v>
       </c>
-      <c r="AE35" s="12">
+      <c r="AI35" s="12">
         <v>7884</v>
       </c>
-      <c r="AF35" s="11">
+      <c r="AJ35" s="11">
         <f t="shared" si="8"/>
         <v>0.87425149700598803</v>
       </c>
-      <c r="AG35" s="12">
+      <c r="AK35" s="12">
         <v>7885</v>
       </c>
-      <c r="AH35" s="13">
+      <c r="AL35" s="13">
         <f t="shared" si="9"/>
         <v>0.87436238633843422</v>
       </c>
-      <c r="AI35">
+      <c r="AM35">
         <v>6585</v>
       </c>
-      <c r="AJ35" s="1">
-        <f t="shared" ref="AJ35:AL35" si="150">AI35/$E35</f>
+      <c r="AN35" s="1">
+        <f t="shared" ref="AN35:AP35" si="150">AM35/$E35</f>
         <v>0.73020625415834994</v>
       </c>
-      <c r="AK35">
+      <c r="AO35">
         <v>6674</v>
       </c>
-      <c r="AL35" s="1">
+      <c r="AP35" s="1">
         <f t="shared" si="150"/>
         <v>0.74007540474606348</v>
       </c>
-      <c r="AM35">
+      <c r="AQ35">
         <v>6777</v>
       </c>
-      <c r="AN35" s="1">
-        <f t="shared" ref="AN35:AP35" si="151">AM35/$E35</f>
+      <c r="AR35" s="1">
+        <f t="shared" ref="AR35:AT35" si="151">AQ35/$E35</f>
         <v>0.75149700598802394</v>
       </c>
-      <c r="AO35">
+      <c r="AS35">
         <v>6633</v>
       </c>
-      <c r="AP35" s="1">
+      <c r="AT35" s="1">
         <f t="shared" si="151"/>
         <v>0.73552894211576847</v>
       </c>
     </row>
-    <row r="36" spans="3:42" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C36">
         <v>30</v>
       </c>
@@ -7601,67 +8442,86 @@
         <f t="shared" ref="W36" si="154">V36/$E36</f>
         <v>0.99412286538035044</v>
       </c>
-      <c r="X36" s="1"/>
-      <c r="Y36" s="1"/>
-      <c r="Z36" s="1"/>
-      <c r="AA36" s="10">
+      <c r="X36" s="24">
+        <v>8959</v>
+      </c>
+      <c r="Y36" s="25">
+        <f>X36/$E36</f>
+        <v>0.99345752938567311</v>
+      </c>
+      <c r="Z36" s="6">
+        <v>8932</v>
+      </c>
+      <c r="AA36" s="25">
+        <f>Z36/$E36</f>
+        <v>0.99046351740962524</v>
+      </c>
+      <c r="AB36">
+        <v>8939</v>
+      </c>
+      <c r="AC36" s="25">
+        <f>AB36/$E36</f>
+        <v>0.99123974273674875</v>
+      </c>
+      <c r="AD36" s="1"/>
+      <c r="AE36" s="10">
         <v>8083</v>
       </c>
-      <c r="AB36" s="11">
+      <c r="AF36" s="11">
         <f t="shared" si="6"/>
         <v>0.89631847416278554</v>
       </c>
-      <c r="AC36" s="12">
+      <c r="AG36" s="12">
         <v>7914</v>
       </c>
-      <c r="AD36" s="11">
+      <c r="AH36" s="11">
         <f t="shared" si="7"/>
         <v>0.87757817697937457</v>
       </c>
-      <c r="AE36" s="12">
+      <c r="AI36" s="12">
         <v>8000</v>
       </c>
-      <c r="AF36" s="11">
+      <c r="AJ36" s="11">
         <f t="shared" si="8"/>
         <v>0.88711465956974944</v>
       </c>
-      <c r="AG36" s="12">
+      <c r="AK36" s="12">
         <v>7913</v>
       </c>
-      <c r="AH36" s="13">
+      <c r="AL36" s="13">
         <f t="shared" si="9"/>
         <v>0.87746728764692838</v>
       </c>
-      <c r="AI36">
+      <c r="AM36">
         <v>7054</v>
       </c>
-      <c r="AJ36" s="1">
-        <f t="shared" ref="AJ36:AL36" si="155">AI36/$E36</f>
+      <c r="AN36" s="1">
+        <f t="shared" ref="AN36:AP36" si="155">AM36/$E36</f>
         <v>0.78221335107562651</v>
       </c>
-      <c r="AK36">
+      <c r="AO36">
         <v>7041</v>
       </c>
-      <c r="AL36" s="1">
+      <c r="AP36" s="1">
         <f t="shared" si="155"/>
         <v>0.78077178975382566</v>
       </c>
-      <c r="AM36">
+      <c r="AQ36">
         <v>6973</v>
       </c>
-      <c r="AN36" s="1">
-        <f t="shared" ref="AN36:AP36" si="156">AM36/$E36</f>
+      <c r="AR36" s="1">
+        <f t="shared" ref="AR36:AT36" si="156">AQ36/$E36</f>
         <v>0.77323131514748278</v>
       </c>
-      <c r="AO36">
+      <c r="AS36">
         <v>6956</v>
       </c>
-      <c r="AP36" s="1">
+      <c r="AT36" s="1">
         <f t="shared" si="156"/>
         <v>0.77134619649589709</v>
       </c>
     </row>
-    <row r="37" spans="3:42" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C37">
         <v>31</v>
       </c>
@@ -7734,67 +8594,86 @@
         <f t="shared" ref="W37" si="159">V37/$E37</f>
         <v>0.99367930805056559</v>
       </c>
-      <c r="X37" s="1"/>
-      <c r="Y37" s="1"/>
-      <c r="Z37" s="1"/>
-      <c r="AA37" s="10">
+      <c r="X37" s="24">
+        <v>8971</v>
+      </c>
+      <c r="Y37" s="25">
+        <f>X37/$E37</f>
+        <v>0.99478820137502777</v>
+      </c>
+      <c r="Z37" s="6">
+        <v>8933</v>
+      </c>
+      <c r="AA37" s="25">
+        <f>Z37/$E37</f>
+        <v>0.99057440674207142</v>
+      </c>
+      <c r="AB37">
+        <v>8939</v>
+      </c>
+      <c r="AC37" s="25">
+        <f>AB37/$E37</f>
+        <v>0.99123974273674875</v>
+      </c>
+      <c r="AD37" s="1"/>
+      <c r="AE37" s="10">
         <v>7855</v>
       </c>
-      <c r="AB37" s="11">
+      <c r="AF37" s="11">
         <f t="shared" si="6"/>
         <v>0.87103570636504768</v>
       </c>
-      <c r="AC37" s="12">
+      <c r="AG37" s="12">
         <v>7638</v>
       </c>
-      <c r="AD37" s="11">
+      <c r="AH37" s="11">
         <f t="shared" si="7"/>
         <v>0.84697272122421818</v>
       </c>
-      <c r="AE37" s="12">
+      <c r="AI37" s="12">
         <v>7682</v>
       </c>
-      <c r="AF37" s="11">
+      <c r="AJ37" s="11">
         <f t="shared" si="8"/>
         <v>0.85185185185185186</v>
       </c>
-      <c r="AG37" s="12">
+      <c r="AK37" s="12">
         <v>7614</v>
       </c>
-      <c r="AH37" s="13">
+      <c r="AL37" s="13">
         <f t="shared" si="9"/>
         <v>0.84431137724550898</v>
       </c>
-      <c r="AI37">
+      <c r="AM37">
         <v>6281</v>
       </c>
-      <c r="AJ37" s="1">
-        <f t="shared" ref="AJ37:AL37" si="160">AI37/$E37</f>
+      <c r="AN37" s="1">
+        <f t="shared" ref="AN37:AP37" si="160">AM37/$E37</f>
         <v>0.6964958970946995</v>
       </c>
-      <c r="AK37">
+      <c r="AO37">
         <v>6385</v>
       </c>
-      <c r="AL37" s="1">
+      <c r="AP37" s="1">
         <f t="shared" si="160"/>
         <v>0.70802838766910625</v>
       </c>
-      <c r="AM37">
+      <c r="AQ37">
         <v>6206</v>
       </c>
-      <c r="AN37" s="1">
-        <f t="shared" ref="AN37:AP37" si="161">AM37/$E37</f>
+      <c r="AR37" s="1">
+        <f t="shared" ref="AR37:AT37" si="161">AQ37/$E37</f>
         <v>0.6881791971612331</v>
       </c>
-      <c r="AO37">
+      <c r="AS37">
         <v>6426</v>
       </c>
-      <c r="AP37" s="1">
+      <c r="AT37" s="1">
         <f t="shared" si="161"/>
         <v>0.71257485029940115</v>
       </c>
     </row>
-    <row r="38" spans="3:42" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C38">
         <v>32</v>
       </c>
@@ -7867,67 +8746,86 @@
         <f t="shared" ref="W38" si="164">V38/$E38</f>
         <v>0.9944555333776891</v>
       </c>
-      <c r="X38" s="1"/>
-      <c r="Y38" s="1"/>
-      <c r="Z38" s="1"/>
-      <c r="AA38" s="10">
+      <c r="X38" s="24">
+        <v>8973</v>
+      </c>
+      <c r="Y38" s="25">
+        <f>X38/$E38</f>
+        <v>0.99500998003992014</v>
+      </c>
+      <c r="Z38" s="6">
+        <v>8932</v>
+      </c>
+      <c r="AA38" s="25">
+        <f>Z38/$E38</f>
+        <v>0.99046351740962524</v>
+      </c>
+      <c r="AB38">
+        <v>8940</v>
+      </c>
+      <c r="AC38" s="25">
+        <f>AB38/$E38</f>
+        <v>0.99135063206919494</v>
+      </c>
+      <c r="AD38" s="1"/>
+      <c r="AE38" s="10">
         <v>7959</v>
       </c>
-      <c r="AB38" s="11">
+      <c r="AF38" s="11">
         <f t="shared" si="6"/>
         <v>0.88256819693945443</v>
       </c>
-      <c r="AC38" s="12">
+      <c r="AG38" s="12">
         <v>7806</v>
       </c>
-      <c r="AD38" s="11">
+      <c r="AH38" s="11">
         <f t="shared" si="7"/>
         <v>0.86560212907518297</v>
       </c>
-      <c r="AE38" s="12">
+      <c r="AI38" s="12">
         <v>7784</v>
       </c>
-      <c r="AF38" s="11">
+      <c r="AJ38" s="11">
         <f t="shared" si="8"/>
         <v>0.86316256376136613</v>
       </c>
-      <c r="AG38" s="12">
+      <c r="AK38" s="12">
         <v>7837</v>
       </c>
-      <c r="AH38" s="13">
+      <c r="AL38" s="13">
         <f t="shared" si="9"/>
         <v>0.8690396983810158</v>
       </c>
-      <c r="AI38">
+      <c r="AM38">
         <v>6727</v>
       </c>
-      <c r="AJ38" s="1">
-        <f t="shared" ref="AJ38:AL39" si="165">AI38/$E38</f>
+      <c r="AN38" s="1">
+        <f t="shared" ref="AN38:AP39" si="165">AM38/$E38</f>
         <v>0.74595253936571304</v>
       </c>
-      <c r="AK38">
+      <c r="AO38">
         <v>6484</v>
       </c>
-      <c r="AL38" s="1">
+      <c r="AP38" s="1">
         <f t="shared" si="165"/>
         <v>0.71900643158128186</v>
       </c>
-      <c r="AM38">
+      <c r="AQ38">
         <v>6610</v>
       </c>
-      <c r="AN38" s="1">
-        <f t="shared" ref="AN38:AP38" si="166">AM38/$E38</f>
+      <c r="AR38" s="1">
+        <f t="shared" ref="AR38:AT38" si="166">AQ38/$E38</f>
         <v>0.73297848746950545</v>
       </c>
-      <c r="AO38">
+      <c r="AS38">
         <v>6590</v>
       </c>
-      <c r="AP38" s="1">
+      <c r="AT38" s="1">
         <f t="shared" si="166"/>
         <v>0.73076070082058109</v>
       </c>
     </row>
-    <row r="39" spans="3:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D39" t="s">
         <v>48</v>
       </c>
@@ -8007,67 +8905,71 @@
         <f>V39/$E39</f>
         <v>0.99719546006729409</v>
       </c>
-      <c r="AA39" s="14">
-        <f>SUM(AA6:AA38)</f>
+      <c r="X39" s="1"/>
+      <c r="Y39" s="1"/>
+      <c r="Z39" s="1"/>
+      <c r="AA39" s="1"/>
+      <c r="AE39" s="14">
+        <f>SUM(AE6:AE38)</f>
         <v>1187199</v>
       </c>
-      <c r="AB39" s="15">
+      <c r="AF39" s="15">
         <f t="shared" si="6"/>
         <v>0.8831689664638025</v>
       </c>
-      <c r="AC39" s="16">
-        <f>SUM(AC6:AC38)</f>
+      <c r="AG39" s="16">
+        <f>SUM(AG6:AG38)</f>
         <v>1156086</v>
       </c>
-      <c r="AD39" s="15">
+      <c r="AH39" s="15">
         <f t="shared" si="7"/>
         <v>0.86002370096611569</v>
       </c>
-      <c r="AE39" s="16">
-        <f>SUM(AE6:AE38)</f>
+      <c r="AI39" s="16">
+        <f>SUM(AI6:AI38)</f>
         <v>1157885</v>
       </c>
-      <c r="AF39" s="15">
+      <c r="AJ39" s="15">
         <f t="shared" si="8"/>
         <v>0.86136199468997188</v>
       </c>
-      <c r="AG39" s="16">
-        <f>SUM(AG6:AG38)</f>
+      <c r="AK39" s="16">
+        <f>SUM(AK6:AK38)</f>
         <v>1155350</v>
       </c>
-      <c r="AH39" s="17">
+      <c r="AL39" s="17">
         <f t="shared" si="9"/>
         <v>0.85947618335591103</v>
       </c>
-      <c r="AI39">
-        <f>SUM(AI6:AI38)</f>
+      <c r="AM39">
+        <f>SUM(AM6:AM38)</f>
         <v>837972</v>
       </c>
-      <c r="AJ39" s="1">
+      <c r="AN39" s="1">
         <f t="shared" si="165"/>
         <v>0.62337557997067505</v>
       </c>
-      <c r="AK39">
-        <f>SUM(AK6:AK38)</f>
+      <c r="AO39">
+        <f>SUM(AO6:AO38)</f>
         <v>835331</v>
       </c>
-      <c r="AL39" s="1">
+      <c r="AP39" s="1">
         <f t="shared" si="165"/>
         <v>0.62141091419818795</v>
       </c>
-      <c r="AM39">
-        <f>SUM(AM6:AM38)</f>
+      <c r="AQ39">
+        <f>SUM(AQ6:AQ38)</f>
         <v>836516</v>
       </c>
-      <c r="AN39" s="1">
-        <f t="shared" ref="AN39:AP39" si="168">AM39/$E39</f>
+      <c r="AR39" s="1">
+        <f t="shared" ref="AR39:AT39" si="168">AQ39/$E39</f>
         <v>0.62229244730700939</v>
       </c>
-      <c r="AO39">
-        <f>SUM(AO6:AO38)</f>
+      <c r="AS39">
+        <f>SUM(AS6:AS38)</f>
         <v>836075</v>
       </c>
-      <c r="AP39" s="1">
+      <c r="AT39" s="1">
         <f t="shared" si="168"/>
         <v>0.62196438308676438</v>
       </c>

</xml_diff>